<commit_message>
make it display only for supervisors. but the condition doesn't work yet
</commit_message>
<xml_diff>
--- a/config/default/forms/contact/person-create.xlsx
+++ b/config/default/forms/contact/person-create.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="333">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -241,6 +241,12 @@
   </si>
   <si>
     <t xml:space="preserve">Nom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ddd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is a test field hardcoded in the db</t>
   </si>
   <si>
     <t xml:space="preserve">end group</t>
@@ -812,6 +818,9 @@
   </si>
   <si>
     <t xml:space="preserve">Create a user for this contact</t>
+  </si>
+  <si>
+    <t xml:space="preserve">../../../inputs/user/ddd = 'chw_supervisor'</t>
   </si>
   <si>
     <t xml:space="preserve">meta</t>
@@ -1593,11 +1602,11 @@
   <dimension ref="A1:AR1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="G8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="J11" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="G1" activeCellId="0" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="K42" activeCellId="0" sqref="K42"/>
+      <selection pane="topRight" activeCell="J1" activeCellId="0" sqref="J1"/>
+      <selection pane="bottomLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+      <selection pane="bottomRight" activeCell="K43" activeCellId="0" sqref="K43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.421875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2036,10 +2045,14 @@
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="12"/>
+      <c r="C7" s="12" t="s">
+        <v>56</v>
+      </c>
       <c r="D7" s="12"/>
       <c r="E7" s="12"/>
       <c r="F7" s="12"/>
@@ -2084,7 +2097,7 @@
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="11" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B8" s="11"/>
       <c r="C8" s="12"/>
@@ -2132,30 +2145,16 @@
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="F9" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="G9" s="12" t="s">
-        <v>33</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="B9" s="11"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
       <c r="H9" s="12"/>
-      <c r="I9" s="12" t="s">
-        <v>33</v>
-      </c>
+      <c r="I9" s="12"/>
       <c r="J9" s="12"/>
       <c r="K9" s="12"/>
       <c r="L9" s="12"/>
@@ -2179,9 +2178,7 @@
       <c r="AD9" s="12"/>
       <c r="AE9" s="12"/>
       <c r="AF9" s="12"/>
-      <c r="AG9" s="12" t="s">
-        <v>57</v>
-      </c>
+      <c r="AG9" s="12"/>
       <c r="AH9" s="12"/>
       <c r="AI9" s="12"/>
       <c r="AJ9" s="12"/>
@@ -2196,38 +2193,34 @@
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="11" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>58</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>60</v>
+        <v>33</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>33</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>61</v>
+        <v>33</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="G10" s="13" t="s">
-        <v>63</v>
+        <v>33</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>33</v>
       </c>
       <c r="H10" s="12"/>
       <c r="I10" s="12" t="s">
-        <v>64</v>
+        <v>33</v>
       </c>
       <c r="J10" s="12"/>
       <c r="K10" s="12"/>
-      <c r="L10" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="M10" s="12" t="s">
-        <v>66</v>
-      </c>
+      <c r="L10" s="12"/>
+      <c r="M10" s="12"/>
       <c r="N10" s="12"/>
       <c r="O10" s="12"/>
       <c r="P10" s="12"/>
@@ -2236,32 +2229,20 @@
       <c r="S10" s="12"/>
       <c r="T10" s="12"/>
       <c r="U10" s="12"/>
-      <c r="V10" s="12" t="s">
-        <v>67</v>
-      </c>
+      <c r="V10" s="12"/>
       <c r="W10" s="12"/>
-      <c r="X10" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="Y10" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="Z10" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="AA10" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="AB10" s="12" t="s">
-        <v>68</v>
-      </c>
+      <c r="X10" s="12"/>
+      <c r="Y10" s="12"/>
+      <c r="Z10" s="12"/>
+      <c r="AA10" s="12"/>
+      <c r="AB10" s="12"/>
       <c r="AC10" s="12"/>
-      <c r="AD10" s="12" t="s">
-        <v>68</v>
-      </c>
+      <c r="AD10" s="12"/>
       <c r="AE10" s="12"/>
       <c r="AF10" s="12"/>
-      <c r="AG10" s="12"/>
+      <c r="AG10" s="12" t="s">
+        <v>59</v>
+      </c>
       <c r="AH10" s="12"/>
       <c r="AI10" s="12"/>
       <c r="AJ10" s="12"/>
@@ -2279,33 +2260,35 @@
         <v>36</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>33</v>
+        <v>61</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>62</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>33</v>
+        <v>63</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="G11" s="12" t="s">
-        <v>33</v>
+        <v>64</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>65</v>
       </c>
       <c r="H11" s="12"/>
       <c r="I11" s="12" t="s">
-        <v>33</v>
+        <v>66</v>
       </c>
       <c r="J11" s="12"/>
       <c r="K11" s="12"/>
       <c r="L11" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="M11" s="12"/>
+        <v>67</v>
+      </c>
+      <c r="M11" s="12" t="s">
+        <v>68</v>
+      </c>
       <c r="N11" s="12"/>
       <c r="O11" s="12"/>
       <c r="P11" s="12"/>
@@ -2314,15 +2297,29 @@
       <c r="S11" s="12"/>
       <c r="T11" s="12"/>
       <c r="U11" s="12"/>
-      <c r="V11" s="12"/>
+      <c r="V11" s="12" t="s">
+        <v>69</v>
+      </c>
       <c r="W11" s="12"/>
-      <c r="X11" s="12"/>
-      <c r="Y11" s="12"/>
-      <c r="Z11" s="12"/>
-      <c r="AA11" s="12"/>
-      <c r="AB11" s="12"/>
+      <c r="X11" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y11" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z11" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="AA11" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="AB11" s="12" t="s">
+        <v>70</v>
+      </c>
       <c r="AC11" s="12"/>
-      <c r="AD11" s="12"/>
+      <c r="AD11" s="12" t="s">
+        <v>70</v>
+      </c>
       <c r="AE11" s="12"/>
       <c r="AF11" s="12"/>
       <c r="AG11" s="12"/>
@@ -2343,7 +2340,7 @@
         <v>36</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C12" s="12" t="s">
         <v>33</v>
@@ -2367,7 +2364,7 @@
       <c r="J12" s="12"/>
       <c r="K12" s="12"/>
       <c r="L12" s="12" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="M12" s="12"/>
       <c r="N12" s="12"/>
@@ -2404,10 +2401,10 @@
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="11" t="s">
-        <v>70</v>
+        <v>36</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>71</v>
+        <v>0</v>
       </c>
       <c r="C13" s="12" t="s">
         <v>33</v>
@@ -2431,7 +2428,7 @@
       <c r="J13" s="12"/>
       <c r="K13" s="12"/>
       <c r="L13" s="12" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="M13" s="12"/>
       <c r="N13" s="12"/>
@@ -2442,9 +2439,7 @@
       <c r="S13" s="12"/>
       <c r="T13" s="12"/>
       <c r="U13" s="12"/>
-      <c r="V13" s="14" t="s">
-        <v>72</v>
-      </c>
+      <c r="V13" s="12"/>
       <c r="W13" s="12"/>
       <c r="X13" s="12"/>
       <c r="Y13" s="12"/>
@@ -2470,21 +2465,35 @@
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="B14" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="B14" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
+      <c r="C14" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>33</v>
+      </c>
       <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
+      <c r="I14" s="12" t="s">
+        <v>33</v>
+      </c>
       <c r="J14" s="12"/>
       <c r="K14" s="12"/>
-      <c r="L14" s="12"/>
+      <c r="L14" s="12" t="s">
+        <v>71</v>
+      </c>
       <c r="M14" s="12"/>
       <c r="N14" s="12"/>
       <c r="O14" s="12"/>
@@ -2494,8 +2503,8 @@
       <c r="S14" s="12"/>
       <c r="T14" s="12"/>
       <c r="U14" s="12"/>
-      <c r="V14" s="12" t="s">
-        <v>75</v>
+      <c r="V14" s="14" t="s">
+        <v>74</v>
       </c>
       <c r="W14" s="12"/>
       <c r="X14" s="12"/>
@@ -2522,9 +2531,11 @@
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="B15" s="11"/>
+        <v>75</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>76</v>
+      </c>
       <c r="C15" s="12"/>
       <c r="D15" s="12"/>
       <c r="E15" s="12"/>
@@ -2544,7 +2555,9 @@
       <c r="S15" s="12"/>
       <c r="T15" s="12"/>
       <c r="U15" s="12"/>
-      <c r="V15" s="12"/>
+      <c r="V15" s="12" t="s">
+        <v>77</v>
+      </c>
       <c r="W15" s="12"/>
       <c r="X15" s="12"/>
       <c r="Y15" s="12"/>
@@ -2569,111 +2582,99 @@
       <c r="AR15" s="12"/>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D16" s="15"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="19"/>
-      <c r="I16" s="20"/>
-      <c r="O16" s="21"/>
-      <c r="P16" s="15"/>
-      <c r="Q16" s="16"/>
-      <c r="R16" s="17"/>
-      <c r="S16" s="18"/>
-      <c r="T16" s="19"/>
-      <c r="U16" s="20"/>
-      <c r="Y16" s="15"/>
-      <c r="Z16" s="16"/>
-      <c r="AA16" s="17"/>
-      <c r="AB16" s="18"/>
-      <c r="AC16" s="19"/>
-      <c r="AD16" s="20"/>
+      <c r="A16" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B16" s="11"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="12"/>
+      <c r="N16" s="12"/>
+      <c r="O16" s="12"/>
+      <c r="P16" s="12"/>
+      <c r="Q16" s="12"/>
+      <c r="R16" s="12"/>
+      <c r="S16" s="12"/>
+      <c r="T16" s="12"/>
+      <c r="U16" s="12"/>
+      <c r="V16" s="12"/>
+      <c r="W16" s="12"/>
+      <c r="X16" s="12"/>
+      <c r="Y16" s="12"/>
+      <c r="Z16" s="12"/>
+      <c r="AA16" s="12"/>
+      <c r="AB16" s="12"/>
+      <c r="AC16" s="12"/>
+      <c r="AD16" s="12"/>
+      <c r="AE16" s="12"/>
+      <c r="AF16" s="12"/>
+      <c r="AG16" s="12"/>
+      <c r="AH16" s="12"/>
+      <c r="AI16" s="12"/>
+      <c r="AJ16" s="12"/>
+      <c r="AK16" s="12"/>
+      <c r="AL16" s="12"/>
+      <c r="AM16" s="12"/>
+      <c r="AN16" s="12"/>
+      <c r="AO16" s="12"/>
+      <c r="AP16" s="12"/>
+      <c r="AQ16" s="12"/>
+      <c r="AR16" s="12"/>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="B17" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="C17" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="D17" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="E17" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="F17" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="G17" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="H17" s="20"/>
-      <c r="I17" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="J17" s="20"/>
-      <c r="K17" s="20"/>
-      <c r="L17" s="20"/>
-      <c r="M17" s="20"/>
-      <c r="N17" s="20"/>
-      <c r="O17" s="20"/>
-      <c r="P17" s="20"/>
-      <c r="Q17" s="20"/>
-      <c r="R17" s="20"/>
-      <c r="S17" s="20"/>
-      <c r="T17" s="20"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="19"/>
+      <c r="I17" s="20"/>
+      <c r="O17" s="21"/>
+      <c r="P17" s="15"/>
+      <c r="Q17" s="16"/>
+      <c r="R17" s="17"/>
+      <c r="S17" s="18"/>
+      <c r="T17" s="19"/>
       <c r="U17" s="20"/>
-      <c r="V17" s="20"/>
-      <c r="W17" s="20"/>
-      <c r="X17" s="20"/>
-      <c r="Y17" s="20"/>
-      <c r="Z17" s="20"/>
-      <c r="AA17" s="20"/>
-      <c r="AB17" s="20"/>
-      <c r="AC17" s="20"/>
+      <c r="Y17" s="15"/>
+      <c r="Z17" s="16"/>
+      <c r="AA17" s="17"/>
+      <c r="AB17" s="18"/>
+      <c r="AC17" s="19"/>
       <c r="AD17" s="20"/>
-      <c r="AE17" s="20"/>
-      <c r="AF17" s="20"/>
-      <c r="AG17" s="20"/>
-      <c r="AH17" s="20"/>
-      <c r="AI17" s="20"/>
-      <c r="AJ17" s="20"/>
-      <c r="AK17" s="20"/>
-      <c r="AL17" s="20"/>
-      <c r="AM17" s="20"/>
-      <c r="AN17" s="20"/>
-      <c r="AO17" s="20"/>
-      <c r="AP17" s="20"/>
-      <c r="AQ17" s="20"/>
-      <c r="AR17" s="20"/>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="22" t="s">
-        <v>69</v>
+        <v>31</v>
       </c>
       <c r="B18" s="22" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C18" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="D18" s="23" t="s">
-        <v>79</v>
+        <v>33</v>
+      </c>
+      <c r="D18" s="20" t="s">
+        <v>33</v>
       </c>
       <c r="E18" s="20" t="s">
-        <v>80</v>
+        <v>33</v>
       </c>
       <c r="F18" s="20" t="s">
-        <v>81</v>
-      </c>
-      <c r="G18" s="20"/>
+        <v>33</v>
+      </c>
+      <c r="G18" s="20" t="s">
+        <v>33</v>
+      </c>
       <c r="H18" s="20"/>
       <c r="I18" s="20" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
       <c r="J18" s="20"/>
       <c r="K18" s="20"/>
@@ -2696,9 +2697,7 @@
       <c r="AB18" s="20"/>
       <c r="AC18" s="20"/>
       <c r="AD18" s="20"/>
-      <c r="AE18" s="20" t="s">
-        <v>83</v>
-      </c>
+      <c r="AE18" s="20"/>
       <c r="AF18" s="20"/>
       <c r="AG18" s="20"/>
       <c r="AH18" s="20"/>
@@ -2715,27 +2714,27 @@
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="22" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B19" s="22" t="s">
-        <v>0</v>
+        <v>79</v>
       </c>
       <c r="C19" s="20" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D19" s="23" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E19" s="20" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F19" s="20" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="G19" s="20"/>
       <c r="H19" s="20"/>
       <c r="I19" s="20" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="J19" s="20"/>
       <c r="K19" s="20"/>
@@ -2759,7 +2758,7 @@
       <c r="AC19" s="20"/>
       <c r="AD19" s="20"/>
       <c r="AE19" s="20" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="AF19" s="20"/>
       <c r="AG19" s="20"/>
@@ -2777,33 +2776,29 @@
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="22" t="s">
-        <v>36</v>
+        <v>71</v>
       </c>
       <c r="B20" s="22" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C20" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="D20" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="E20" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="F20" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="D20" s="23" t="s">
-        <v>90</v>
-      </c>
-      <c r="E20" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="F20" s="20" t="s">
-        <v>92</v>
-      </c>
-      <c r="G20" s="23" t="s">
-        <v>90</v>
-      </c>
+      <c r="G20" s="20"/>
       <c r="H20" s="20"/>
       <c r="I20" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="J20" s="20" t="s">
-        <v>93</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="J20" s="20"/>
       <c r="K20" s="20"/>
       <c r="L20" s="20"/>
       <c r="M20" s="20"/>
@@ -2824,7 +2819,9 @@
       <c r="AB20" s="20"/>
       <c r="AC20" s="20"/>
       <c r="AD20" s="20"/>
-      <c r="AE20" s="20"/>
+      <c r="AE20" s="20" t="s">
+        <v>78</v>
+      </c>
       <c r="AF20" s="20"/>
       <c r="AG20" s="20"/>
       <c r="AH20" s="20"/>
@@ -2844,29 +2841,35 @@
         <v>36</v>
       </c>
       <c r="B21" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="D21" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="E21" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="F21" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="C21" s="20" t="s">
+      <c r="G21" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="H21" s="20"/>
+      <c r="I21" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="J21" s="20" t="s">
         <v>95</v>
-      </c>
-      <c r="D21" s="20"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="20"/>
-      <c r="I21" s="20"/>
-      <c r="J21" s="20" t="s">
-        <v>96</v>
       </c>
       <c r="K21" s="20"/>
       <c r="L21" s="20"/>
       <c r="M21" s="20"/>
-      <c r="N21" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="O21" s="20" t="s">
-        <v>98</v>
-      </c>
+      <c r="N21" s="20"/>
+      <c r="O21" s="20"/>
       <c r="P21" s="20"/>
       <c r="Q21" s="20"/>
       <c r="R21" s="20"/>
@@ -2875,9 +2878,7 @@
       <c r="U21" s="20"/>
       <c r="V21" s="20"/>
       <c r="W21" s="20"/>
-      <c r="X21" s="24" t="s">
-        <v>99</v>
-      </c>
+      <c r="X21" s="20"/>
       <c r="Y21" s="20"/>
       <c r="Z21" s="20"/>
       <c r="AA21" s="20"/>
@@ -2901,37 +2902,43 @@
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="22" t="s">
-        <v>73</v>
+        <v>36</v>
       </c>
       <c r="B22" s="22" t="s">
-        <v>100</v>
-      </c>
-      <c r="C22" s="25"/>
-      <c r="D22" s="25"/>
-      <c r="E22" s="25"/>
-      <c r="F22" s="25"/>
-      <c r="G22" s="25"/>
+        <v>96</v>
+      </c>
+      <c r="C22" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20"/>
       <c r="H22" s="20"/>
-      <c r="I22" s="25"/>
+      <c r="I22" s="20"/>
       <c r="J22" s="20" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="K22" s="20"/>
       <c r="L22" s="20"/>
       <c r="M22" s="20"/>
-      <c r="N22" s="20"/>
-      <c r="O22" s="20"/>
+      <c r="N22" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="O22" s="20" t="s">
+        <v>100</v>
+      </c>
       <c r="P22" s="20"/>
       <c r="Q22" s="20"/>
       <c r="R22" s="20"/>
       <c r="S22" s="20"/>
       <c r="T22" s="20"/>
       <c r="U22" s="20"/>
-      <c r="V22" s="20" t="s">
+      <c r="V22" s="20"/>
+      <c r="W22" s="20"/>
+      <c r="X22" s="24" t="s">
         <v>101</v>
       </c>
-      <c r="W22" s="20"/>
-      <c r="X22" s="20"/>
       <c r="Y22" s="20"/>
       <c r="Z22" s="20"/>
       <c r="AA22" s="20"/>
@@ -2955,19 +2962,21 @@
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="22" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B23" s="22" t="s">
         <v>102</v>
       </c>
       <c r="C23" s="25"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="20"/>
+      <c r="D23" s="25"/>
+      <c r="E23" s="25"/>
+      <c r="F23" s="25"/>
+      <c r="G23" s="25"/>
       <c r="H23" s="20"/>
-      <c r="I23" s="20"/>
-      <c r="J23" s="20"/>
+      <c r="I23" s="25"/>
+      <c r="J23" s="20" t="s">
+        <v>95</v>
+      </c>
       <c r="K23" s="20"/>
       <c r="L23" s="20"/>
       <c r="M23" s="20"/>
@@ -3007,14 +3016,12 @@
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="22" t="s">
-        <v>31</v>
+        <v>75</v>
       </c>
       <c r="B24" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="C24" s="20" t="s">
-        <v>33</v>
-      </c>
+      <c r="C24" s="25"/>
       <c r="D24" s="20"/>
       <c r="E24" s="20"/>
       <c r="F24" s="20"/>
@@ -3033,7 +3040,9 @@
       <c r="S24" s="20"/>
       <c r="T24" s="20"/>
       <c r="U24" s="20"/>
-      <c r="V24" s="20"/>
+      <c r="V24" s="20" t="s">
+        <v>105</v>
+      </c>
       <c r="W24" s="20"/>
       <c r="X24" s="20"/>
       <c r="Y24" s="20"/>
@@ -3059,13 +3068,13 @@
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="22" t="s">
-        <v>105</v>
+        <v>31</v>
       </c>
       <c r="B25" s="22" t="s">
         <v>106</v>
       </c>
       <c r="C25" s="20" t="s">
-        <v>107</v>
+        <v>33</v>
       </c>
       <c r="D25" s="20"/>
       <c r="E25" s="20"/>
@@ -3073,20 +3082,12 @@
       <c r="G25" s="20"/>
       <c r="H25" s="20"/>
       <c r="I25" s="20"/>
-      <c r="J25" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="K25" s="20" t="s">
-        <v>108</v>
-      </c>
+      <c r="J25" s="20"/>
+      <c r="K25" s="20"/>
       <c r="L25" s="20"/>
       <c r="M25" s="20"/>
-      <c r="N25" s="20" t="s">
-        <v>109</v>
-      </c>
-      <c r="O25" s="20" t="s">
-        <v>110</v>
-      </c>
+      <c r="N25" s="20"/>
+      <c r="O25" s="20"/>
       <c r="P25" s="20"/>
       <c r="Q25" s="20"/>
       <c r="R25" s="20"/>
@@ -3095,9 +3096,7 @@
       <c r="U25" s="20"/>
       <c r="V25" s="20"/>
       <c r="W25" s="20"/>
-      <c r="X25" s="20" t="s">
-        <v>111</v>
-      </c>
+      <c r="X25" s="20"/>
       <c r="Y25" s="20"/>
       <c r="Z25" s="20"/>
       <c r="AA25" s="20"/>
@@ -3121,13 +3120,13 @@
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="22" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="B26" s="22" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="C26" s="20" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D26" s="20"/>
       <c r="E26" s="20"/>
@@ -3135,14 +3134,20 @@
       <c r="G26" s="20"/>
       <c r="H26" s="20"/>
       <c r="I26" s="20"/>
-      <c r="J26" s="20"/>
+      <c r="J26" s="20" t="s">
+        <v>95</v>
+      </c>
       <c r="K26" s="20" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="L26" s="20"/>
       <c r="M26" s="20"/>
-      <c r="N26" s="20"/>
-      <c r="O26" s="20"/>
+      <c r="N26" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="O26" s="20" t="s">
+        <v>112</v>
+      </c>
       <c r="P26" s="20"/>
       <c r="Q26" s="20"/>
       <c r="R26" s="20"/>
@@ -3151,7 +3156,9 @@
       <c r="U26" s="20"/>
       <c r="V26" s="20"/>
       <c r="W26" s="20"/>
-      <c r="X26" s="20"/>
+      <c r="X26" s="20" t="s">
+        <v>113</v>
+      </c>
       <c r="Y26" s="20"/>
       <c r="Z26" s="20"/>
       <c r="AA26" s="20"/>
@@ -3175,13 +3182,13 @@
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="22" t="s">
+        <v>114</v>
+      </c>
+      <c r="B27" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="C27" s="20" t="s">
         <v>116</v>
-      </c>
-      <c r="B27" s="22" t="s">
-        <v>117</v>
-      </c>
-      <c r="C27" s="20" t="s">
-        <v>118</v>
       </c>
       <c r="D27" s="20"/>
       <c r="E27" s="20"/>
@@ -3189,20 +3196,14 @@
       <c r="G27" s="20"/>
       <c r="H27" s="20"/>
       <c r="I27" s="20"/>
-      <c r="J27" s="20" t="s">
-        <v>93</v>
-      </c>
+      <c r="J27" s="20"/>
       <c r="K27" s="20" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="L27" s="20"/>
       <c r="M27" s="20"/>
-      <c r="N27" s="20" t="s">
-        <v>119</v>
-      </c>
-      <c r="O27" s="20" t="s">
-        <v>120</v>
-      </c>
+      <c r="N27" s="20"/>
+      <c r="O27" s="20"/>
       <c r="P27" s="20"/>
       <c r="Q27" s="20"/>
       <c r="R27" s="20"/>
@@ -3235,13 +3236,13 @@
     </row>
     <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="22" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B28" s="22" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C28" s="20" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D28" s="20"/>
       <c r="E28" s="20"/>
@@ -3249,17 +3250,19 @@
       <c r="G28" s="20"/>
       <c r="H28" s="20"/>
       <c r="I28" s="20"/>
-      <c r="J28" s="20"/>
+      <c r="J28" s="20" t="s">
+        <v>95</v>
+      </c>
       <c r="K28" s="20" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="L28" s="20"/>
       <c r="M28" s="20"/>
       <c r="N28" s="20" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="O28" s="20" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="P28" s="20"/>
       <c r="Q28" s="20"/>
@@ -3293,13 +3296,13 @@
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="22" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="B29" s="22" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C29" s="20" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D29" s="20"/>
       <c r="E29" s="20"/>
@@ -3308,13 +3311,17 @@
       <c r="H29" s="20"/>
       <c r="I29" s="20"/>
       <c r="J29" s="20"/>
-      <c r="K29" s="20"/>
-      <c r="L29" s="20" t="s">
-        <v>128</v>
-      </c>
+      <c r="K29" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="L29" s="20"/>
       <c r="M29" s="20"/>
-      <c r="N29" s="20"/>
-      <c r="O29" s="20"/>
+      <c r="N29" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="O29" s="20" t="s">
+        <v>126</v>
+      </c>
       <c r="P29" s="20"/>
       <c r="Q29" s="20"/>
       <c r="R29" s="20"/>
@@ -3347,12 +3354,14 @@
     </row>
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="22" t="s">
-        <v>73</v>
+        <v>127</v>
       </c>
       <c r="B30" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="C30" s="20" t="s">
         <v>129</v>
       </c>
-      <c r="C30" s="25"/>
       <c r="D30" s="20"/>
       <c r="E30" s="20"/>
       <c r="F30" s="20"/>
@@ -3361,7 +3370,9 @@
       <c r="I30" s="20"/>
       <c r="J30" s="20"/>
       <c r="K30" s="20"/>
-      <c r="L30" s="20"/>
+      <c r="L30" s="20" t="s">
+        <v>130</v>
+      </c>
       <c r="M30" s="20"/>
       <c r="N30" s="20"/>
       <c r="O30" s="20"/>
@@ -3371,9 +3382,7 @@
       <c r="S30" s="20"/>
       <c r="T30" s="20"/>
       <c r="U30" s="20"/>
-      <c r="V30" s="25" t="s">
-        <v>130</v>
-      </c>
+      <c r="V30" s="20"/>
       <c r="W30" s="20"/>
       <c r="X30" s="20"/>
       <c r="Y30" s="20"/>
@@ -3399,12 +3408,12 @@
     </row>
     <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="22" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B31" s="22" t="s">
         <v>131</v>
       </c>
-      <c r="C31" s="20"/>
+      <c r="C31" s="25"/>
       <c r="D31" s="20"/>
       <c r="E31" s="20"/>
       <c r="F31" s="20"/>
@@ -3421,9 +3430,9 @@
       <c r="Q31" s="20"/>
       <c r="R31" s="20"/>
       <c r="S31" s="20"/>
-      <c r="T31" s="25"/>
+      <c r="T31" s="20"/>
       <c r="U31" s="20"/>
-      <c r="V31" s="26" t="s">
+      <c r="V31" s="25" t="s">
         <v>132</v>
       </c>
       <c r="W31" s="20"/>
@@ -3451,12 +3460,12 @@
     </row>
     <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="22" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B32" s="22" t="s">
         <v>133</v>
       </c>
-      <c r="C32" s="25"/>
+      <c r="C32" s="20"/>
       <c r="D32" s="20"/>
       <c r="E32" s="20"/>
       <c r="F32" s="20"/>
@@ -3473,9 +3482,9 @@
       <c r="Q32" s="20"/>
       <c r="R32" s="20"/>
       <c r="S32" s="20"/>
-      <c r="T32" s="20"/>
+      <c r="T32" s="25"/>
       <c r="U32" s="20"/>
-      <c r="V32" s="20" t="s">
+      <c r="V32" s="26" t="s">
         <v>134</v>
       </c>
       <c r="W32" s="20"/>
@@ -3503,14 +3512,12 @@
     </row>
     <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="22" t="s">
-        <v>112</v>
+        <v>75</v>
       </c>
       <c r="B33" s="22" t="s">
         <v>135</v>
       </c>
-      <c r="C33" s="27" t="s">
-        <v>136</v>
-      </c>
+      <c r="C33" s="25"/>
       <c r="D33" s="20"/>
       <c r="E33" s="20"/>
       <c r="F33" s="20"/>
@@ -3518,9 +3525,7 @@
       <c r="H33" s="20"/>
       <c r="I33" s="20"/>
       <c r="J33" s="20"/>
-      <c r="K33" s="20" t="s">
-        <v>34</v>
-      </c>
+      <c r="K33" s="20"/>
       <c r="L33" s="20"/>
       <c r="M33" s="20"/>
       <c r="N33" s="20"/>
@@ -3531,7 +3536,9 @@
       <c r="S33" s="20"/>
       <c r="T33" s="20"/>
       <c r="U33" s="20"/>
-      <c r="V33" s="20"/>
+      <c r="V33" s="20" t="s">
+        <v>136</v>
+      </c>
       <c r="W33" s="20"/>
       <c r="X33" s="20"/>
       <c r="Y33" s="20"/>
@@ -3557,10 +3564,14 @@
     </row>
     <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="B34" s="22"/>
-      <c r="C34" s="20"/>
+        <v>114</v>
+      </c>
+      <c r="B34" s="22" t="s">
+        <v>137</v>
+      </c>
+      <c r="C34" s="27" t="s">
+        <v>138</v>
+      </c>
       <c r="D34" s="20"/>
       <c r="E34" s="20"/>
       <c r="F34" s="20"/>
@@ -3568,7 +3579,9 @@
       <c r="H34" s="20"/>
       <c r="I34" s="20"/>
       <c r="J34" s="20"/>
-      <c r="K34" s="20"/>
+      <c r="K34" s="20" t="s">
+        <v>34</v>
+      </c>
       <c r="L34" s="20"/>
       <c r="M34" s="20"/>
       <c r="N34" s="20"/>
@@ -3605,37 +3618,19 @@
     </row>
     <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="22" t="s">
-        <v>137</v>
-      </c>
-      <c r="B35" s="22" t="s">
-        <v>138</v>
-      </c>
-      <c r="C35" s="20" t="s">
-        <v>139</v>
-      </c>
-      <c r="D35" s="23" t="s">
-        <v>140</v>
-      </c>
-      <c r="E35" s="20" t="s">
-        <v>141</v>
-      </c>
-      <c r="F35" s="20" t="s">
-        <v>142</v>
-      </c>
-      <c r="G35" s="23" t="s">
-        <v>140</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="B35" s="22"/>
+      <c r="C35" s="20"/>
+      <c r="D35" s="20"/>
+      <c r="E35" s="20"/>
+      <c r="F35" s="20"/>
+      <c r="G35" s="20"/>
       <c r="H35" s="20"/>
-      <c r="I35" s="20" t="s">
-        <v>143</v>
-      </c>
-      <c r="J35" s="20" t="s">
-        <v>93</v>
-      </c>
+      <c r="I35" s="20"/>
+      <c r="J35" s="20"/>
       <c r="K35" s="20"/>
-      <c r="L35" s="20" t="s">
-        <v>128</v>
-      </c>
+      <c r="L35" s="20"/>
       <c r="M35" s="20"/>
       <c r="N35" s="20"/>
       <c r="O35" s="20"/>
@@ -3671,50 +3666,46 @@
     </row>
     <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="22" t="s">
+        <v>139</v>
+      </c>
+      <c r="B36" s="22" t="s">
+        <v>140</v>
+      </c>
+      <c r="C36" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="D36" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="E36" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="F36" s="20" t="s">
         <v>144</v>
       </c>
-      <c r="B36" s="22" t="s">
-        <v>145</v>
-      </c>
-      <c r="C36" s="20" t="s">
-        <v>146</v>
-      </c>
-      <c r="D36" s="23" t="s">
-        <v>147</v>
-      </c>
-      <c r="E36" s="20" t="s">
-        <v>148</v>
-      </c>
-      <c r="F36" s="20" t="s">
-        <v>149</v>
-      </c>
       <c r="G36" s="23" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="H36" s="20"/>
       <c r="I36" s="20" t="s">
-        <v>151</v>
-      </c>
-      <c r="J36" s="20"/>
+        <v>145</v>
+      </c>
+      <c r="J36" s="20" t="s">
+        <v>95</v>
+      </c>
       <c r="K36" s="20"/>
-      <c r="L36" s="20"/>
+      <c r="L36" s="20" t="s">
+        <v>130</v>
+      </c>
       <c r="M36" s="20"/>
-      <c r="N36" s="20" t="s">
-        <v>152</v>
-      </c>
-      <c r="O36" s="20" t="s">
-        <v>153</v>
-      </c>
-      <c r="P36" s="28" t="s">
-        <v>154</v>
-      </c>
+      <c r="N36" s="20"/>
+      <c r="O36" s="20"/>
+      <c r="P36" s="20"/>
       <c r="Q36" s="20"/>
       <c r="R36" s="20"/>
       <c r="S36" s="20"/>
       <c r="T36" s="20"/>
-      <c r="U36" s="20" t="s">
-        <v>155</v>
-      </c>
+      <c r="U36" s="20"/>
       <c r="V36" s="20"/>
       <c r="W36" s="20"/>
       <c r="X36" s="20"/>
@@ -3741,49 +3732,49 @@
     </row>
     <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="22" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B37" s="22" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="C37" s="20" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="D37" s="23" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="E37" s="20" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="F37" s="20" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="G37" s="23" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="H37" s="20"/>
       <c r="I37" s="20" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="J37" s="20"/>
       <c r="K37" s="20"/>
       <c r="L37" s="20"/>
       <c r="M37" s="20"/>
       <c r="N37" s="20" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="O37" s="20" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="P37" s="28" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="Q37" s="20"/>
       <c r="R37" s="20"/>
       <c r="S37" s="20"/>
       <c r="T37" s="20"/>
       <c r="U37" s="20" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="V37" s="20"/>
       <c r="W37" s="20"/>
@@ -3811,63 +3802,59 @@
     </row>
     <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="22" t="s">
+        <v>146</v>
+      </c>
+      <c r="B38" s="22" t="s">
+        <v>158</v>
+      </c>
+      <c r="C38" s="20" t="s">
+        <v>159</v>
+      </c>
+      <c r="D38" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="E38" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="F38" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="G38" s="23" t="s">
         <v>163</v>
-      </c>
-      <c r="B38" s="22" t="s">
-        <v>164</v>
-      </c>
-      <c r="C38" s="20" t="s">
-        <v>165</v>
-      </c>
-      <c r="D38" s="23" t="s">
-        <v>166</v>
-      </c>
-      <c r="E38" s="20" t="s">
-        <v>167</v>
-      </c>
-      <c r="F38" s="20" t="s">
-        <v>168</v>
-      </c>
-      <c r="G38" s="23" t="s">
-        <v>166</v>
       </c>
       <c r="H38" s="20"/>
       <c r="I38" s="20" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="J38" s="20"/>
       <c r="K38" s="20"/>
       <c r="L38" s="20"/>
       <c r="M38" s="20"/>
-      <c r="N38" s="20"/>
-      <c r="O38" s="20"/>
-      <c r="P38" s="20"/>
+      <c r="N38" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="O38" s="20" t="s">
+        <v>155</v>
+      </c>
+      <c r="P38" s="28" t="s">
+        <v>156</v>
+      </c>
       <c r="Q38" s="20"/>
       <c r="R38" s="20"/>
       <c r="S38" s="20"/>
       <c r="T38" s="20"/>
-      <c r="U38" s="20"/>
+      <c r="U38" s="20" t="s">
+        <v>157</v>
+      </c>
       <c r="V38" s="20"/>
       <c r="W38" s="20"/>
-      <c r="X38" s="20" t="s">
-        <v>170</v>
-      </c>
-      <c r="Y38" s="23" t="s">
-        <v>171</v>
-      </c>
-      <c r="Z38" s="20" t="s">
-        <v>172</v>
-      </c>
-      <c r="AA38" s="20" t="s">
-        <v>173</v>
-      </c>
-      <c r="AB38" s="23" t="s">
-        <v>174</v>
-      </c>
+      <c r="X38" s="20"/>
+      <c r="Y38" s="20"/>
+      <c r="Z38" s="20"/>
+      <c r="AA38" s="20"/>
+      <c r="AB38" s="20"/>
       <c r="AC38" s="20"/>
-      <c r="AD38" s="20" t="s">
-        <v>175</v>
-      </c>
+      <c r="AD38" s="20"/>
       <c r="AE38" s="20"/>
       <c r="AF38" s="20"/>
       <c r="AG38" s="20"/>
@@ -3885,36 +3872,32 @@
     </row>
     <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="22" t="s">
-        <v>36</v>
+        <v>165</v>
       </c>
       <c r="B39" s="22" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="C39" s="20" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="D39" s="23" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="E39" s="20" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="F39" s="20" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="G39" s="23" t="s">
-        <v>181</v>
+        <v>168</v>
       </c>
       <c r="H39" s="20"/>
       <c r="I39" s="20" t="s">
-        <v>182</v>
-      </c>
-      <c r="J39" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="K39" s="20" t="s">
-        <v>183</v>
-      </c>
+        <v>171</v>
+      </c>
+      <c r="J39" s="20"/>
+      <c r="K39" s="20"/>
       <c r="L39" s="20"/>
       <c r="M39" s="20"/>
       <c r="N39" s="20"/>
@@ -3927,13 +3910,25 @@
       <c r="U39" s="20"/>
       <c r="V39" s="20"/>
       <c r="W39" s="20"/>
-      <c r="X39" s="20"/>
-      <c r="Y39" s="20"/>
-      <c r="Z39" s="20"/>
-      <c r="AA39" s="20"/>
-      <c r="AB39" s="20"/>
+      <c r="X39" s="20" t="s">
+        <v>172</v>
+      </c>
+      <c r="Y39" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="Z39" s="20" t="s">
+        <v>174</v>
+      </c>
+      <c r="AA39" s="20" t="s">
+        <v>175</v>
+      </c>
+      <c r="AB39" s="23" t="s">
+        <v>176</v>
+      </c>
       <c r="AC39" s="20"/>
-      <c r="AD39" s="20"/>
+      <c r="AD39" s="20" t="s">
+        <v>177</v>
+      </c>
       <c r="AE39" s="20"/>
       <c r="AF39" s="20"/>
       <c r="AG39" s="20"/>
@@ -3954,29 +3949,33 @@
         <v>36</v>
       </c>
       <c r="B40" s="22" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="C40" s="20" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="D40" s="23" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="E40" s="20" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="F40" s="20" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="G40" s="23" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="H40" s="20"/>
       <c r="I40" s="20" t="s">
-        <v>190</v>
-      </c>
-      <c r="J40" s="20"/>
-      <c r="K40" s="20"/>
+        <v>184</v>
+      </c>
+      <c r="J40" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="K40" s="20" t="s">
+        <v>185</v>
+      </c>
       <c r="L40" s="20"/>
       <c r="M40" s="20"/>
       <c r="N40" s="20"/>
@@ -4016,22 +4015,22 @@
         <v>36</v>
       </c>
       <c r="B41" s="22" t="s">
+        <v>186</v>
+      </c>
+      <c r="C41" s="20" t="s">
+        <v>187</v>
+      </c>
+      <c r="D41" s="23" t="s">
+        <v>188</v>
+      </c>
+      <c r="E41" s="20" t="s">
+        <v>189</v>
+      </c>
+      <c r="F41" s="20" t="s">
+        <v>190</v>
+      </c>
+      <c r="G41" s="23" t="s">
         <v>191</v>
-      </c>
-      <c r="C41" s="20" t="s">
-        <v>192</v>
-      </c>
-      <c r="D41" s="23" t="s">
-        <v>193</v>
-      </c>
-      <c r="E41" s="20" t="s">
-        <v>194</v>
-      </c>
-      <c r="F41" s="20" t="s">
-        <v>195</v>
-      </c>
-      <c r="G41" s="23" t="s">
-        <v>196</v>
       </c>
       <c r="H41" s="20"/>
       <c r="I41" s="20" t="s">
@@ -4039,9 +4038,7 @@
       </c>
       <c r="J41" s="20"/>
       <c r="K41" s="20"/>
-      <c r="L41" s="20" t="s">
-        <v>197</v>
-      </c>
+      <c r="L41" s="20"/>
       <c r="M41" s="20"/>
       <c r="N41" s="20"/>
       <c r="O41" s="20"/>
@@ -4077,26 +4074,34 @@
     </row>
     <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="B42" s="22" t="s">
+        <v>193</v>
+      </c>
+      <c r="C42" s="20" t="s">
+        <v>194</v>
+      </c>
+      <c r="D42" s="23" t="s">
+        <v>195</v>
+      </c>
+      <c r="E42" s="20" t="s">
+        <v>196</v>
+      </c>
+      <c r="F42" s="20" t="s">
+        <v>197</v>
+      </c>
+      <c r="G42" s="23" t="s">
         <v>198</v>
       </c>
-      <c r="B42" s="22" t="s">
-        <v>199</v>
-      </c>
-      <c r="C42" s="20" t="s">
-        <v>200</v>
-      </c>
-      <c r="D42" s="20"/>
-      <c r="E42" s="20"/>
-      <c r="F42" s="20"/>
-      <c r="G42" s="20"/>
       <c r="H42" s="20"/>
-      <c r="I42" s="20"/>
-      <c r="J42" s="20" t="s">
-        <v>93</v>
-      </c>
+      <c r="I42" s="20" t="s">
+        <v>194</v>
+      </c>
+      <c r="J42" s="20"/>
       <c r="K42" s="20"/>
       <c r="L42" s="20" t="s">
-        <v>128</v>
+        <v>199</v>
       </c>
       <c r="M42" s="20"/>
       <c r="N42" s="20"/>
@@ -4133,34 +4138,28 @@
     </row>
     <row r="43" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="22" t="s">
-        <v>31</v>
+        <v>200</v>
       </c>
       <c r="B43" s="22" t="s">
         <v>201</v>
       </c>
       <c r="C43" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="D43" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="E43" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="F43" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="G43" s="20" t="s">
-        <v>33</v>
-      </c>
+        <v>202</v>
+      </c>
+      <c r="D43" s="20"/>
+      <c r="E43" s="20"/>
+      <c r="F43" s="20"/>
+      <c r="G43" s="20"/>
       <c r="H43" s="20"/>
-      <c r="I43" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="J43" s="20"/>
-      <c r="K43" s="20"/>
+      <c r="I43" s="20"/>
+      <c r="J43" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="K43" s="20" t="s">
+        <v>203</v>
+      </c>
       <c r="L43" s="20" t="s">
-        <v>69</v>
+        <v>130</v>
       </c>
       <c r="M43" s="20"/>
       <c r="N43" s="20"/>
@@ -4197,21 +4196,35 @@
     </row>
     <row r="44" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="22" t="s">
-        <v>73</v>
+        <v>31</v>
       </c>
       <c r="B44" s="22" t="s">
-        <v>202</v>
-      </c>
-      <c r="C44" s="20"/>
-      <c r="D44" s="20"/>
-      <c r="E44" s="20"/>
-      <c r="F44" s="20"/>
-      <c r="G44" s="20"/>
+        <v>204</v>
+      </c>
+      <c r="C44" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="D44" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="E44" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="F44" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="G44" s="20" t="s">
+        <v>33</v>
+      </c>
       <c r="H44" s="20"/>
-      <c r="I44" s="20"/>
+      <c r="I44" s="20" t="s">
+        <v>33</v>
+      </c>
       <c r="J44" s="20"/>
       <c r="K44" s="20"/>
-      <c r="L44" s="20"/>
+      <c r="L44" s="20" t="s">
+        <v>71</v>
+      </c>
       <c r="M44" s="20"/>
       <c r="N44" s="20"/>
       <c r="O44" s="20"/>
@@ -4221,9 +4234,7 @@
       <c r="S44" s="20"/>
       <c r="T44" s="20"/>
       <c r="U44" s="20"/>
-      <c r="V44" s="20" t="s">
-        <v>203</v>
-      </c>
+      <c r="V44" s="20"/>
       <c r="W44" s="20"/>
       <c r="X44" s="20"/>
       <c r="Y44" s="20"/>
@@ -4249,10 +4260,10 @@
     </row>
     <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="22" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B45" s="22" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C45" s="20"/>
       <c r="D45" s="20"/>
@@ -4274,7 +4285,7 @@
       <c r="T45" s="20"/>
       <c r="U45" s="20"/>
       <c r="V45" s="20" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="W45" s="20"/>
       <c r="X45" s="20"/>
@@ -4301,10 +4312,10 @@
     </row>
     <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="22" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B46" s="22" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C46" s="20"/>
       <c r="D46" s="20"/>
@@ -4326,7 +4337,7 @@
       <c r="T46" s="20"/>
       <c r="U46" s="20"/>
       <c r="V46" s="20" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="W46" s="20"/>
       <c r="X46" s="20"/>
@@ -4353,9 +4364,11 @@
     </row>
     <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="B47" s="22"/>
+        <v>75</v>
+      </c>
+      <c r="B47" s="22" t="s">
+        <v>209</v>
+      </c>
       <c r="C47" s="20"/>
       <c r="D47" s="20"/>
       <c r="E47" s="20"/>
@@ -4375,7 +4388,9 @@
       <c r="S47" s="20"/>
       <c r="T47" s="20"/>
       <c r="U47" s="20"/>
-      <c r="V47" s="20"/>
+      <c r="V47" s="20" t="s">
+        <v>210</v>
+      </c>
       <c r="W47" s="20"/>
       <c r="X47" s="20"/>
       <c r="Y47" s="20"/>
@@ -4401,7 +4416,7 @@
     </row>
     <row r="48" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="22" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B48" s="22"/>
       <c r="C48" s="20"/>
@@ -4447,7 +4462,54 @@
       <c r="AQ48" s="20"/>
       <c r="AR48" s="20"/>
     </row>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="49" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A49" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="B49" s="22"/>
+      <c r="C49" s="20"/>
+      <c r="D49" s="20"/>
+      <c r="E49" s="20"/>
+      <c r="F49" s="20"/>
+      <c r="G49" s="20"/>
+      <c r="H49" s="20"/>
+      <c r="I49" s="20"/>
+      <c r="J49" s="20"/>
+      <c r="K49" s="20"/>
+      <c r="L49" s="20"/>
+      <c r="M49" s="20"/>
+      <c r="N49" s="20"/>
+      <c r="O49" s="20"/>
+      <c r="P49" s="20"/>
+      <c r="Q49" s="20"/>
+      <c r="R49" s="20"/>
+      <c r="S49" s="20"/>
+      <c r="T49" s="20"/>
+      <c r="U49" s="20"/>
+      <c r="V49" s="20"/>
+      <c r="W49" s="20"/>
+      <c r="X49" s="20"/>
+      <c r="Y49" s="20"/>
+      <c r="Z49" s="20"/>
+      <c r="AA49" s="20"/>
+      <c r="AB49" s="20"/>
+      <c r="AC49" s="20"/>
+      <c r="AD49" s="20"/>
+      <c r="AE49" s="20"/>
+      <c r="AF49" s="20"/>
+      <c r="AG49" s="20"/>
+      <c r="AH49" s="20"/>
+      <c r="AI49" s="20"/>
+      <c r="AJ49" s="20"/>
+      <c r="AK49" s="20"/>
+      <c r="AL49" s="20"/>
+      <c r="AM49" s="20"/>
+      <c r="AN49" s="20"/>
+      <c r="AO49" s="20"/>
+      <c r="AP49" s="20"/>
+      <c r="AQ49" s="20"/>
+      <c r="AR49" s="20"/>
+    </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -4488,7 +4550,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="29" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="B1" s="29" t="s">
         <v>1</v>
@@ -4517,434 +4579,434 @@
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="30" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C2" s="30" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="D2" s="31" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="G2" s="32" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="H2" s="19"/>
       <c r="I2" s="20" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="30" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="C3" s="30" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="D3" s="31" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="F3" s="17" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="G3" s="32" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="H3" s="19"/>
       <c r="I3" s="20" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="30" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="D4" s="33" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="G4" s="32" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="H4" s="19"/>
       <c r="I4" s="20" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="30" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="D5" s="33" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="G5" s="32" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="H5" s="19"/>
       <c r="I5" s="20" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="30" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="B6" s="30" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="D6" s="33" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="F6" s="17" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="G6" s="32" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="H6" s="19"/>
       <c r="I6" s="20" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="30" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="B7" s="30" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="D7" s="33" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="F7" s="17" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="G7" s="32" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="H7" s="19"/>
       <c r="I7" s="20" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="B8" s="34" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="C8" s="35" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="D8" s="33" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="G8" s="32" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="H8" s="19"/>
       <c r="I8" s="20" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="B9" s="34" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="C9" s="35" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="D9" s="33" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="F9" s="17" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="G9" s="32" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="H9" s="19"/>
       <c r="I9" s="20" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="B10" s="34" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="C10" s="35" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="D10" s="33" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="F10" s="17" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="G10" s="32" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="H10" s="19"/>
       <c r="I10" s="20" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="B11" s="34" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="C11" s="35" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="D11" s="33" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="F11" s="17" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="G11" s="32" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="H11" s="19"/>
       <c r="I11" s="20" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="B12" s="34" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="C12" s="35" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="D12" s="33" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="F12" s="17" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="G12" s="36" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="H12" s="19"/>
       <c r="I12" s="20" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D13" s="31" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="E13" s="16" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="F13" s="17" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="G13" s="32" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="H13" s="19"/>
       <c r="I13" s="20" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="B14" s="34" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="C14" s="35" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="D14" s="31" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="E14" s="16" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="F14" s="17" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="G14" s="32" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="H14" s="19"/>
       <c r="I14" s="20" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="B15" s="34" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="C15" s="35" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="D15" s="31" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="E15" s="16" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="F15" s="17" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="G15" s="32" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="H15" s="19"/>
       <c r="I15" s="20" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="B16" s="34" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="C16" s="35" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="E16" s="16" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="F16" s="17" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="G16" s="32" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="H16" s="19"/>
       <c r="I16" s="20" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="B17" s="34" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="C17" s="35" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="E17" s="16" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="F17" s="17" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="G17" s="32" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="H17" s="19"/>
       <c r="I17" s="20" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
     </row>
   </sheetData>
@@ -4979,40 +5041,40 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="C2" s="37" t="str">
         <f aca="true">TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2022-12-15  14-26</v>
+        <v>2022-12-15  16-46</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
make it display the "create associated user" field only when creating contacts with "chw" or "chw_supervisor" roles
</commit_message>
<xml_diff>
--- a/config/default/forms/contact/person-create.xlsx
+++ b/config/default/forms/contact/person-create.xlsx
@@ -150,6 +150,7 @@
         <color rgb="FF000000"/>
         <rFont val="Droid Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">लग इन गरेको प्रयोगकर्ताको सम्पर्क </t>
     </r>
@@ -180,6 +181,7 @@
         <color rgb="FF000000"/>
         <rFont val="Droid Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">लॉग इन यूज़र के स्थान का </t>
     </r>
@@ -207,6 +209,7 @@
         <color rgb="FF000000"/>
         <rFont val="Droid Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">लग इन गरेको प्रयोगकर्ताको स्थानको </t>
     </r>
@@ -327,6 +330,7 @@
         <color rgb="FF000000"/>
         <rFont val="Droid Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">मूल </t>
     </r>
@@ -574,6 +578,7 @@
         <color rgb="FF000000"/>
         <rFont val="Droid Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">कृपया एक सही स्थानीय नंबर दर्ज करें</t>
     </r>
@@ -593,6 +598,7 @@
         <color rgb="FF000000"/>
         <rFont val="Droid Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">या मानक अंतरराष्ट्रीय प्रारूप का उपयोग करें</t>
     </r>
@@ -612,6 +618,7 @@
         <color rgb="FF000000"/>
         <rFont val="Droid Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">जिसमें एक प्लस साइन </t>
     </r>
@@ -631,6 +638,7 @@
         <color rgb="FF000000"/>
         <rFont val="Droid Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">और देश कोड शामिल है। उदाहरण के लिए</t>
     </r>
@@ -745,6 +753,7 @@
         <color rgb="FF000000"/>
         <rFont val="Droid Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">बाहरी </t>
     </r>
@@ -772,6 +781,7 @@
         <color rgb="FF000000"/>
         <rFont val="Droid Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">बाहिरी </t>
     </r>
@@ -820,7 +830,7 @@
     <t xml:space="preserve">Create a user for this contact</t>
   </si>
   <si>
-    <t xml:space="preserve">../../../inputs/user/ddd = 'chw_supervisor'</t>
+    <t xml:space="preserve">selected( ${role},'chw') or selected( ${role},'chw_supervisor')</t>
   </si>
   <si>
     <t xml:space="preserve">meta</t>
@@ -1253,6 +1263,7 @@
       <color rgb="FF000000"/>
       <name val="Droid Sans Devanagari"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1606,10 +1617,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="J1" activeCellId="0" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="K43" activeCellId="0" sqref="K43"/>
+      <selection pane="bottomRight" activeCell="K44" activeCellId="0" sqref="K44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.421875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.40625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.43"/>
@@ -4533,7 +4544,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.421875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.40625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.29"/>
@@ -5031,7 +5042,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.421875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.40625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="7.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.43"/>
@@ -5068,7 +5079,7 @@
       </c>
       <c r="C2" s="37" t="str">
         <f aca="true">TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2022-12-15  16-46</v>
+        <v>2022-12-19  11-00</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>331</v>

</xml_diff>

<commit_message>
calculate the `should_create_user` property
</commit_message>
<xml_diff>
--- a/config/default/forms/contact/person-create.xlsx
+++ b/config/default/forms/contact/person-create.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="333">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -830,7 +830,7 @@
     <t xml:space="preserve">Create a user for this contact</t>
   </si>
   <si>
-    <t xml:space="preserve">selected( ${role},'chw') or selected( ${role},'chw_supervisor')</t>
+    <t xml:space="preserve">if(selected( ${role},'chw') or selected( ${role},'chw_supervisor'), 'true', 'false')</t>
   </si>
   <si>
     <t xml:space="preserve">meta</t>
@@ -1613,14 +1613,14 @@
   <dimension ref="A1:AR1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="J11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="V11" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="J1" activeCellId="0" sqref="J1"/>
+      <selection pane="topRight" activeCell="V1" activeCellId="0" sqref="V1"/>
       <selection pane="bottomLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="K44" activeCellId="0" sqref="K44"/>
+      <selection pane="bottomRight" activeCell="V44" activeCellId="0" sqref="V44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.40625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.390625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.43"/>
@@ -4166,13 +4166,13 @@
       <c r="J43" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="K43" s="20" t="s">
-        <v>203</v>
-      </c>
+      <c r="K43" s="20"/>
       <c r="L43" s="20" t="s">
-        <v>130</v>
-      </c>
-      <c r="M43" s="20"/>
+        <v>71</v>
+      </c>
+      <c r="M43" s="20" t="s">
+        <v>68</v>
+      </c>
       <c r="N43" s="20"/>
       <c r="O43" s="20"/>
       <c r="P43" s="20"/>
@@ -4181,7 +4181,9 @@
       <c r="S43" s="20"/>
       <c r="T43" s="20"/>
       <c r="U43" s="20"/>
-      <c r="V43" s="20"/>
+      <c r="V43" s="20" t="s">
+        <v>203</v>
+      </c>
       <c r="W43" s="20"/>
       <c r="X43" s="20"/>
       <c r="Y43" s="20"/>
@@ -4544,7 +4546,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.40625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.390625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.29"/>
@@ -5042,7 +5044,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.40625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.390625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="7.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.43"/>
@@ -5079,7 +5081,7 @@
       </c>
       <c r="C2" s="37" t="str">
         <f aca="true">TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2022-12-19  11-00</v>
+        <v>2022-12-22  12-22</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>331</v>

</xml_diff>

<commit_message>
remove unnecessary `ddd` field
</commit_message>
<xml_diff>
--- a/config/default/forms/contact/person-create.xlsx
+++ b/config/default/forms/contact/person-create.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="331">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -244,12 +244,6 @@
   </si>
   <si>
     <t xml:space="preserve">Nom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ddd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This is a test field hardcoded in the db</t>
   </si>
   <si>
     <t xml:space="preserve">end group</t>
@@ -1613,14 +1607,14 @@
   <dimension ref="A1:AR1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="V11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="V2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="V1" activeCellId="0" sqref="V1"/>
-      <selection pane="bottomLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="V44" activeCellId="0" sqref="V44"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.390625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.43"/>
@@ -2056,14 +2050,10 @@
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B7" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="C7" s="12" t="s">
-        <v>56</v>
-      </c>
+      <c r="B7" s="11"/>
+      <c r="C7" s="12"/>
       <c r="D7" s="12"/>
       <c r="E7" s="12"/>
       <c r="F7" s="12"/>
@@ -2108,7 +2098,7 @@
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B8" s="11"/>
       <c r="C8" s="12"/>
@@ -2156,16 +2146,30 @@
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="B9" s="11"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
+        <v>31</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>33</v>
+      </c>
       <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
+      <c r="I9" s="12" t="s">
+        <v>33</v>
+      </c>
       <c r="J9" s="12"/>
       <c r="K9" s="12"/>
       <c r="L9" s="12"/>
@@ -2189,7 +2193,9 @@
       <c r="AD9" s="12"/>
       <c r="AE9" s="12"/>
       <c r="AF9" s="12"/>
-      <c r="AG9" s="12"/>
+      <c r="AG9" s="12" t="s">
+        <v>57</v>
+      </c>
       <c r="AH9" s="12"/>
       <c r="AI9" s="12"/>
       <c r="AJ9" s="12"/>
@@ -2204,34 +2210,38 @@
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="11" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>58</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>33</v>
+        <v>59</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>60</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>33</v>
+        <v>61</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="G10" s="12" t="s">
-        <v>33</v>
+        <v>62</v>
+      </c>
+      <c r="G10" s="13" t="s">
+        <v>63</v>
       </c>
       <c r="H10" s="12"/>
       <c r="I10" s="12" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="J10" s="12"/>
       <c r="K10" s="12"/>
-      <c r="L10" s="12"/>
-      <c r="M10" s="12"/>
+      <c r="L10" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="M10" s="12" t="s">
+        <v>66</v>
+      </c>
       <c r="N10" s="12"/>
       <c r="O10" s="12"/>
       <c r="P10" s="12"/>
@@ -2240,20 +2250,32 @@
       <c r="S10" s="12"/>
       <c r="T10" s="12"/>
       <c r="U10" s="12"/>
-      <c r="V10" s="12"/>
+      <c r="V10" s="12" t="s">
+        <v>67</v>
+      </c>
       <c r="W10" s="12"/>
-      <c r="X10" s="12"/>
-      <c r="Y10" s="12"/>
-      <c r="Z10" s="12"/>
-      <c r="AA10" s="12"/>
-      <c r="AB10" s="12"/>
+      <c r="X10" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y10" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z10" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA10" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB10" s="12" t="s">
+        <v>68</v>
+      </c>
       <c r="AC10" s="12"/>
-      <c r="AD10" s="12"/>
+      <c r="AD10" s="12" t="s">
+        <v>68</v>
+      </c>
       <c r="AE10" s="12"/>
       <c r="AF10" s="12"/>
-      <c r="AG10" s="12" t="s">
-        <v>59</v>
-      </c>
+      <c r="AG10" s="12"/>
       <c r="AH10" s="12"/>
       <c r="AI10" s="12"/>
       <c r="AJ10" s="12"/>
@@ -2271,35 +2293,33 @@
         <v>36</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>60</v>
+        <v>1</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>62</v>
+        <v>33</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>33</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>63</v>
+        <v>33</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="G11" s="13" t="s">
-        <v>65</v>
+        <v>33</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>33</v>
       </c>
       <c r="H11" s="12"/>
       <c r="I11" s="12" t="s">
-        <v>66</v>
+        <v>33</v>
       </c>
       <c r="J11" s="12"/>
       <c r="K11" s="12"/>
       <c r="L11" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="M11" s="12" t="s">
-        <v>68</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="M11" s="12"/>
       <c r="N11" s="12"/>
       <c r="O11" s="12"/>
       <c r="P11" s="12"/>
@@ -2308,29 +2328,15 @@
       <c r="S11" s="12"/>
       <c r="T11" s="12"/>
       <c r="U11" s="12"/>
-      <c r="V11" s="12" t="s">
-        <v>69</v>
-      </c>
+      <c r="V11" s="12"/>
       <c r="W11" s="12"/>
-      <c r="X11" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="Y11" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="Z11" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="AA11" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="AB11" s="12" t="s">
-        <v>70</v>
-      </c>
+      <c r="X11" s="12"/>
+      <c r="Y11" s="12"/>
+      <c r="Z11" s="12"/>
+      <c r="AA11" s="12"/>
+      <c r="AB11" s="12"/>
       <c r="AC11" s="12"/>
-      <c r="AD11" s="12" t="s">
-        <v>70</v>
-      </c>
+      <c r="AD11" s="12"/>
       <c r="AE11" s="12"/>
       <c r="AF11" s="12"/>
       <c r="AG11" s="12"/>
@@ -2351,7 +2357,7 @@
         <v>36</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C12" s="12" t="s">
         <v>33</v>
@@ -2375,7 +2381,7 @@
       <c r="J12" s="12"/>
       <c r="K12" s="12"/>
       <c r="L12" s="12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="M12" s="12"/>
       <c r="N12" s="12"/>
@@ -2412,10 +2418,10 @@
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="11" t="s">
-        <v>36</v>
+        <v>70</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>0</v>
+        <v>71</v>
       </c>
       <c r="C13" s="12" t="s">
         <v>33</v>
@@ -2439,7 +2445,7 @@
       <c r="J13" s="12"/>
       <c r="K13" s="12"/>
       <c r="L13" s="12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="M13" s="12"/>
       <c r="N13" s="12"/>
@@ -2450,7 +2456,9 @@
       <c r="S13" s="12"/>
       <c r="T13" s="12"/>
       <c r="U13" s="12"/>
-      <c r="V13" s="12"/>
+      <c r="V13" s="14" t="s">
+        <v>72</v>
+      </c>
       <c r="W13" s="12"/>
       <c r="X13" s="12"/>
       <c r="Y13" s="12"/>
@@ -2476,35 +2484,21 @@
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="11" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="E14" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="F14" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="G14" s="12" t="s">
-        <v>33</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
       <c r="H14" s="12"/>
-      <c r="I14" s="12" t="s">
-        <v>33</v>
-      </c>
+      <c r="I14" s="12"/>
       <c r="J14" s="12"/>
       <c r="K14" s="12"/>
-      <c r="L14" s="12" t="s">
-        <v>71</v>
-      </c>
+      <c r="L14" s="12"/>
       <c r="M14" s="12"/>
       <c r="N14" s="12"/>
       <c r="O14" s="12"/>
@@ -2514,8 +2508,8 @@
       <c r="S14" s="12"/>
       <c r="T14" s="12"/>
       <c r="U14" s="12"/>
-      <c r="V14" s="14" t="s">
-        <v>74</v>
+      <c r="V14" s="12" t="s">
+        <v>75</v>
       </c>
       <c r="W14" s="12"/>
       <c r="X14" s="12"/>
@@ -2542,11 +2536,9 @@
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>76</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="B15" s="11"/>
       <c r="C15" s="12"/>
       <c r="D15" s="12"/>
       <c r="E15" s="12"/>
@@ -2566,9 +2558,7 @@
       <c r="S15" s="12"/>
       <c r="T15" s="12"/>
       <c r="U15" s="12"/>
-      <c r="V15" s="12" t="s">
-        <v>77</v>
-      </c>
+      <c r="V15" s="12"/>
       <c r="W15" s="12"/>
       <c r="X15" s="12"/>
       <c r="Y15" s="12"/>
@@ -2593,99 +2583,111 @@
       <c r="AR15" s="12"/>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="B16" s="11"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="12"/>
-      <c r="K16" s="12"/>
-      <c r="L16" s="12"/>
-      <c r="M16" s="12"/>
-      <c r="N16" s="12"/>
-      <c r="O16" s="12"/>
-      <c r="P16" s="12"/>
-      <c r="Q16" s="12"/>
-      <c r="R16" s="12"/>
-      <c r="S16" s="12"/>
-      <c r="T16" s="12"/>
-      <c r="U16" s="12"/>
-      <c r="V16" s="12"/>
-      <c r="W16" s="12"/>
-      <c r="X16" s="12"/>
-      <c r="Y16" s="12"/>
-      <c r="Z16" s="12"/>
-      <c r="AA16" s="12"/>
-      <c r="AB16" s="12"/>
-      <c r="AC16" s="12"/>
-      <c r="AD16" s="12"/>
-      <c r="AE16" s="12"/>
-      <c r="AF16" s="12"/>
-      <c r="AG16" s="12"/>
-      <c r="AH16" s="12"/>
-      <c r="AI16" s="12"/>
-      <c r="AJ16" s="12"/>
-      <c r="AK16" s="12"/>
-      <c r="AL16" s="12"/>
-      <c r="AM16" s="12"/>
-      <c r="AN16" s="12"/>
-      <c r="AO16" s="12"/>
-      <c r="AP16" s="12"/>
-      <c r="AQ16" s="12"/>
-      <c r="AR16" s="12"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="20"/>
+      <c r="O16" s="21"/>
+      <c r="P16" s="15"/>
+      <c r="Q16" s="16"/>
+      <c r="R16" s="17"/>
+      <c r="S16" s="18"/>
+      <c r="T16" s="19"/>
+      <c r="U16" s="20"/>
+      <c r="Y16" s="15"/>
+      <c r="Z16" s="16"/>
+      <c r="AA16" s="17"/>
+      <c r="AB16" s="18"/>
+      <c r="AC16" s="19"/>
+      <c r="AD16" s="20"/>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D17" s="15"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="19"/>
-      <c r="I17" s="20"/>
-      <c r="O17" s="21"/>
-      <c r="P17" s="15"/>
-      <c r="Q17" s="16"/>
-      <c r="R17" s="17"/>
-      <c r="S17" s="18"/>
-      <c r="T17" s="19"/>
+      <c r="A17" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="C17" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="F17" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="G17" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="H17" s="20"/>
+      <c r="I17" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="J17" s="20"/>
+      <c r="K17" s="20"/>
+      <c r="L17" s="20"/>
+      <c r="M17" s="20"/>
+      <c r="N17" s="20"/>
+      <c r="O17" s="20"/>
+      <c r="P17" s="20"/>
+      <c r="Q17" s="20"/>
+      <c r="R17" s="20"/>
+      <c r="S17" s="20"/>
+      <c r="T17" s="20"/>
       <c r="U17" s="20"/>
-      <c r="Y17" s="15"/>
-      <c r="Z17" s="16"/>
-      <c r="AA17" s="17"/>
-      <c r="AB17" s="18"/>
-      <c r="AC17" s="19"/>
+      <c r="V17" s="20"/>
+      <c r="W17" s="20"/>
+      <c r="X17" s="20"/>
+      <c r="Y17" s="20"/>
+      <c r="Z17" s="20"/>
+      <c r="AA17" s="20"/>
+      <c r="AB17" s="20"/>
+      <c r="AC17" s="20"/>
       <c r="AD17" s="20"/>
+      <c r="AE17" s="20"/>
+      <c r="AF17" s="20"/>
+      <c r="AG17" s="20"/>
+      <c r="AH17" s="20"/>
+      <c r="AI17" s="20"/>
+      <c r="AJ17" s="20"/>
+      <c r="AK17" s="20"/>
+      <c r="AL17" s="20"/>
+      <c r="AM17" s="20"/>
+      <c r="AN17" s="20"/>
+      <c r="AO17" s="20"/>
+      <c r="AP17" s="20"/>
+      <c r="AQ17" s="20"/>
+      <c r="AR17" s="20"/>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="22" t="s">
-        <v>31</v>
+        <v>69</v>
       </c>
       <c r="B18" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="C18" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="C18" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="D18" s="20" t="s">
-        <v>33</v>
+      <c r="D18" s="23" t="s">
+        <v>79</v>
       </c>
       <c r="E18" s="20" t="s">
-        <v>33</v>
+        <v>80</v>
       </c>
       <c r="F18" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="G18" s="20" t="s">
-        <v>33</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="G18" s="20"/>
       <c r="H18" s="20"/>
       <c r="I18" s="20" t="s">
-        <v>33</v>
+        <v>82</v>
       </c>
       <c r="J18" s="20"/>
       <c r="K18" s="20"/>
@@ -2708,7 +2710,9 @@
       <c r="AB18" s="20"/>
       <c r="AC18" s="20"/>
       <c r="AD18" s="20"/>
-      <c r="AE18" s="20"/>
+      <c r="AE18" s="20" t="s">
+        <v>83</v>
+      </c>
       <c r="AF18" s="20"/>
       <c r="AG18" s="20"/>
       <c r="AH18" s="20"/>
@@ -2725,27 +2729,27 @@
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="22" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B19" s="22" t="s">
-        <v>79</v>
+        <v>0</v>
       </c>
       <c r="C19" s="20" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="D19" s="23" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="E19" s="20" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="F19" s="20" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="G19" s="20"/>
       <c r="H19" s="20"/>
       <c r="I19" s="20" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="J19" s="20"/>
       <c r="K19" s="20"/>
@@ -2769,7 +2773,7 @@
       <c r="AC19" s="20"/>
       <c r="AD19" s="20"/>
       <c r="AE19" s="20" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="AF19" s="20"/>
       <c r="AG19" s="20"/>
@@ -2787,29 +2791,33 @@
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="22" t="s">
-        <v>71</v>
+        <v>36</v>
       </c>
       <c r="B20" s="22" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C20" s="20" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="D20" s="23" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="E20" s="20" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="F20" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="G20" s="20"/>
+        <v>92</v>
+      </c>
+      <c r="G20" s="23" t="s">
+        <v>90</v>
+      </c>
       <c r="H20" s="20"/>
       <c r="I20" s="20" t="s">
-        <v>90</v>
-      </c>
-      <c r="J20" s="20"/>
+        <v>54</v>
+      </c>
+      <c r="J20" s="20" t="s">
+        <v>93</v>
+      </c>
       <c r="K20" s="20"/>
       <c r="L20" s="20"/>
       <c r="M20" s="20"/>
@@ -2830,9 +2838,7 @@
       <c r="AB20" s="20"/>
       <c r="AC20" s="20"/>
       <c r="AD20" s="20"/>
-      <c r="AE20" s="20" t="s">
-        <v>78</v>
-      </c>
+      <c r="AE20" s="20"/>
       <c r="AF20" s="20"/>
       <c r="AG20" s="20"/>
       <c r="AH20" s="20"/>
@@ -2852,35 +2858,29 @@
         <v>36</v>
       </c>
       <c r="B21" s="22" t="s">
-        <v>1</v>
+        <v>94</v>
       </c>
       <c r="C21" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="D21" s="23" t="s">
-        <v>92</v>
-      </c>
-      <c r="E21" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="F21" s="20" t="s">
-        <v>94</v>
-      </c>
-      <c r="G21" s="23" t="s">
-        <v>92</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20"/>
       <c r="H21" s="20"/>
-      <c r="I21" s="20" t="s">
-        <v>54</v>
-      </c>
+      <c r="I21" s="20"/>
       <c r="J21" s="20" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="K21" s="20"/>
       <c r="L21" s="20"/>
       <c r="M21" s="20"/>
-      <c r="N21" s="20"/>
-      <c r="O21" s="20"/>
+      <c r="N21" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="O21" s="20" t="s">
+        <v>98</v>
+      </c>
       <c r="P21" s="20"/>
       <c r="Q21" s="20"/>
       <c r="R21" s="20"/>
@@ -2889,7 +2889,9 @@
       <c r="U21" s="20"/>
       <c r="V21" s="20"/>
       <c r="W21" s="20"/>
-      <c r="X21" s="20"/>
+      <c r="X21" s="24" t="s">
+        <v>99</v>
+      </c>
       <c r="Y21" s="20"/>
       <c r="Z21" s="20"/>
       <c r="AA21" s="20"/>
@@ -2913,43 +2915,37 @@
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="22" t="s">
-        <v>36</v>
+        <v>73</v>
       </c>
       <c r="B22" s="22" t="s">
-        <v>96</v>
-      </c>
-      <c r="C22" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="D22" s="20"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="20"/>
-      <c r="G22" s="20"/>
+        <v>100</v>
+      </c>
+      <c r="C22" s="25"/>
+      <c r="D22" s="25"/>
+      <c r="E22" s="25"/>
+      <c r="F22" s="25"/>
+      <c r="G22" s="25"/>
       <c r="H22" s="20"/>
-      <c r="I22" s="20"/>
+      <c r="I22" s="25"/>
       <c r="J22" s="20" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="K22" s="20"/>
       <c r="L22" s="20"/>
       <c r="M22" s="20"/>
-      <c r="N22" s="20" t="s">
-        <v>99</v>
-      </c>
-      <c r="O22" s="20" t="s">
-        <v>100</v>
-      </c>
+      <c r="N22" s="20"/>
+      <c r="O22" s="20"/>
       <c r="P22" s="20"/>
       <c r="Q22" s="20"/>
       <c r="R22" s="20"/>
       <c r="S22" s="20"/>
       <c r="T22" s="20"/>
       <c r="U22" s="20"/>
-      <c r="V22" s="20"/>
+      <c r="V22" s="20" t="s">
+        <v>101</v>
+      </c>
       <c r="W22" s="20"/>
-      <c r="X22" s="24" t="s">
-        <v>101</v>
-      </c>
+      <c r="X22" s="20"/>
       <c r="Y22" s="20"/>
       <c r="Z22" s="20"/>
       <c r="AA22" s="20"/>
@@ -2973,21 +2969,19 @@
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="22" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B23" s="22" t="s">
         <v>102</v>
       </c>
       <c r="C23" s="25"/>
-      <c r="D23" s="25"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="25"/>
-      <c r="G23" s="25"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="20"/>
       <c r="H23" s="20"/>
-      <c r="I23" s="25"/>
-      <c r="J23" s="20" t="s">
-        <v>95</v>
-      </c>
+      <c r="I23" s="20"/>
+      <c r="J23" s="20"/>
       <c r="K23" s="20"/>
       <c r="L23" s="20"/>
       <c r="M23" s="20"/>
@@ -3027,12 +3021,14 @@
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="22" t="s">
-        <v>75</v>
+        <v>31</v>
       </c>
       <c r="B24" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="C24" s="25"/>
+      <c r="C24" s="20" t="s">
+        <v>33</v>
+      </c>
       <c r="D24" s="20"/>
       <c r="E24" s="20"/>
       <c r="F24" s="20"/>
@@ -3051,9 +3047,7 @@
       <c r="S24" s="20"/>
       <c r="T24" s="20"/>
       <c r="U24" s="20"/>
-      <c r="V24" s="20" t="s">
-        <v>105</v>
-      </c>
+      <c r="V24" s="20"/>
       <c r="W24" s="20"/>
       <c r="X24" s="20"/>
       <c r="Y24" s="20"/>
@@ -3079,13 +3073,13 @@
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="22" t="s">
-        <v>31</v>
+        <v>105</v>
       </c>
       <c r="B25" s="22" t="s">
         <v>106</v>
       </c>
       <c r="C25" s="20" t="s">
-        <v>33</v>
+        <v>107</v>
       </c>
       <c r="D25" s="20"/>
       <c r="E25" s="20"/>
@@ -3093,12 +3087,20 @@
       <c r="G25" s="20"/>
       <c r="H25" s="20"/>
       <c r="I25" s="20"/>
-      <c r="J25" s="20"/>
-      <c r="K25" s="20"/>
+      <c r="J25" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="K25" s="20" t="s">
+        <v>108</v>
+      </c>
       <c r="L25" s="20"/>
       <c r="M25" s="20"/>
-      <c r="N25" s="20"/>
-      <c r="O25" s="20"/>
+      <c r="N25" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="O25" s="20" t="s">
+        <v>110</v>
+      </c>
       <c r="P25" s="20"/>
       <c r="Q25" s="20"/>
       <c r="R25" s="20"/>
@@ -3107,7 +3109,9 @@
       <c r="U25" s="20"/>
       <c r="V25" s="20"/>
       <c r="W25" s="20"/>
-      <c r="X25" s="20"/>
+      <c r="X25" s="20" t="s">
+        <v>111</v>
+      </c>
       <c r="Y25" s="20"/>
       <c r="Z25" s="20"/>
       <c r="AA25" s="20"/>
@@ -3131,13 +3135,13 @@
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="22" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="B26" s="22" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="C26" s="20" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="D26" s="20"/>
       <c r="E26" s="20"/>
@@ -3145,20 +3149,14 @@
       <c r="G26" s="20"/>
       <c r="H26" s="20"/>
       <c r="I26" s="20"/>
-      <c r="J26" s="20" t="s">
-        <v>95</v>
-      </c>
+      <c r="J26" s="20"/>
       <c r="K26" s="20" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="L26" s="20"/>
       <c r="M26" s="20"/>
-      <c r="N26" s="20" t="s">
-        <v>111</v>
-      </c>
-      <c r="O26" s="20" t="s">
-        <v>112</v>
-      </c>
+      <c r="N26" s="20"/>
+      <c r="O26" s="20"/>
       <c r="P26" s="20"/>
       <c r="Q26" s="20"/>
       <c r="R26" s="20"/>
@@ -3167,9 +3165,7 @@
       <c r="U26" s="20"/>
       <c r="V26" s="20"/>
       <c r="W26" s="20"/>
-      <c r="X26" s="20" t="s">
-        <v>113</v>
-      </c>
+      <c r="X26" s="20"/>
       <c r="Y26" s="20"/>
       <c r="Z26" s="20"/>
       <c r="AA26" s="20"/>
@@ -3193,13 +3189,13 @@
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="22" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B27" s="22" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C27" s="20" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="D27" s="20"/>
       <c r="E27" s="20"/>
@@ -3207,14 +3203,20 @@
       <c r="G27" s="20"/>
       <c r="H27" s="20"/>
       <c r="I27" s="20"/>
-      <c r="J27" s="20"/>
+      <c r="J27" s="20" t="s">
+        <v>93</v>
+      </c>
       <c r="K27" s="20" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="L27" s="20"/>
       <c r="M27" s="20"/>
-      <c r="N27" s="20"/>
-      <c r="O27" s="20"/>
+      <c r="N27" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="O27" s="20" t="s">
+        <v>120</v>
+      </c>
       <c r="P27" s="20"/>
       <c r="Q27" s="20"/>
       <c r="R27" s="20"/>
@@ -3247,13 +3249,13 @@
     </row>
     <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="22" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B28" s="22" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C28" s="20" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="D28" s="20"/>
       <c r="E28" s="20"/>
@@ -3261,19 +3263,17 @@
       <c r="G28" s="20"/>
       <c r="H28" s="20"/>
       <c r="I28" s="20"/>
-      <c r="J28" s="20" t="s">
-        <v>95</v>
-      </c>
+      <c r="J28" s="20"/>
       <c r="K28" s="20" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="L28" s="20"/>
       <c r="M28" s="20"/>
       <c r="N28" s="20" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="O28" s="20" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="P28" s="20"/>
       <c r="Q28" s="20"/>
@@ -3307,13 +3307,13 @@
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="22" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="B29" s="22" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="C29" s="20" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="D29" s="20"/>
       <c r="E29" s="20"/>
@@ -3322,17 +3322,13 @@
       <c r="H29" s="20"/>
       <c r="I29" s="20"/>
       <c r="J29" s="20"/>
-      <c r="K29" s="20" t="s">
-        <v>117</v>
-      </c>
-      <c r="L29" s="20"/>
+      <c r="K29" s="20"/>
+      <c r="L29" s="20" t="s">
+        <v>128</v>
+      </c>
       <c r="M29" s="20"/>
-      <c r="N29" s="20" t="s">
-        <v>125</v>
-      </c>
-      <c r="O29" s="20" t="s">
-        <v>126</v>
-      </c>
+      <c r="N29" s="20"/>
+      <c r="O29" s="20"/>
       <c r="P29" s="20"/>
       <c r="Q29" s="20"/>
       <c r="R29" s="20"/>
@@ -3365,14 +3361,12 @@
     </row>
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="22" t="s">
-        <v>127</v>
+        <v>73</v>
       </c>
       <c r="B30" s="22" t="s">
-        <v>128</v>
-      </c>
-      <c r="C30" s="20" t="s">
         <v>129</v>
       </c>
+      <c r="C30" s="25"/>
       <c r="D30" s="20"/>
       <c r="E30" s="20"/>
       <c r="F30" s="20"/>
@@ -3381,9 +3375,7 @@
       <c r="I30" s="20"/>
       <c r="J30" s="20"/>
       <c r="K30" s="20"/>
-      <c r="L30" s="20" t="s">
-        <v>130</v>
-      </c>
+      <c r="L30" s="20"/>
       <c r="M30" s="20"/>
       <c r="N30" s="20"/>
       <c r="O30" s="20"/>
@@ -3393,7 +3385,9 @@
       <c r="S30" s="20"/>
       <c r="T30" s="20"/>
       <c r="U30" s="20"/>
-      <c r="V30" s="20"/>
+      <c r="V30" s="25" t="s">
+        <v>130</v>
+      </c>
       <c r="W30" s="20"/>
       <c r="X30" s="20"/>
       <c r="Y30" s="20"/>
@@ -3419,12 +3413,12 @@
     </row>
     <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="22" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B31" s="22" t="s">
         <v>131</v>
       </c>
-      <c r="C31" s="25"/>
+      <c r="C31" s="20"/>
       <c r="D31" s="20"/>
       <c r="E31" s="20"/>
       <c r="F31" s="20"/>
@@ -3441,9 +3435,9 @@
       <c r="Q31" s="20"/>
       <c r="R31" s="20"/>
       <c r="S31" s="20"/>
-      <c r="T31" s="20"/>
+      <c r="T31" s="25"/>
       <c r="U31" s="20"/>
-      <c r="V31" s="25" t="s">
+      <c r="V31" s="26" t="s">
         <v>132</v>
       </c>
       <c r="W31" s="20"/>
@@ -3471,12 +3465,12 @@
     </row>
     <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="22" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B32" s="22" t="s">
         <v>133</v>
       </c>
-      <c r="C32" s="20"/>
+      <c r="C32" s="25"/>
       <c r="D32" s="20"/>
       <c r="E32" s="20"/>
       <c r="F32" s="20"/>
@@ -3493,9 +3487,9 @@
       <c r="Q32" s="20"/>
       <c r="R32" s="20"/>
       <c r="S32" s="20"/>
-      <c r="T32" s="25"/>
+      <c r="T32" s="20"/>
       <c r="U32" s="20"/>
-      <c r="V32" s="26" t="s">
+      <c r="V32" s="20" t="s">
         <v>134</v>
       </c>
       <c r="W32" s="20"/>
@@ -3523,12 +3517,14 @@
     </row>
     <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="22" t="s">
-        <v>75</v>
+        <v>112</v>
       </c>
       <c r="B33" s="22" t="s">
         <v>135</v>
       </c>
-      <c r="C33" s="25"/>
+      <c r="C33" s="27" t="s">
+        <v>136</v>
+      </c>
       <c r="D33" s="20"/>
       <c r="E33" s="20"/>
       <c r="F33" s="20"/>
@@ -3536,7 +3532,9 @@
       <c r="H33" s="20"/>
       <c r="I33" s="20"/>
       <c r="J33" s="20"/>
-      <c r="K33" s="20"/>
+      <c r="K33" s="20" t="s">
+        <v>34</v>
+      </c>
       <c r="L33" s="20"/>
       <c r="M33" s="20"/>
       <c r="N33" s="20"/>
@@ -3547,9 +3545,7 @@
       <c r="S33" s="20"/>
       <c r="T33" s="20"/>
       <c r="U33" s="20"/>
-      <c r="V33" s="20" t="s">
-        <v>136</v>
-      </c>
+      <c r="V33" s="20"/>
       <c r="W33" s="20"/>
       <c r="X33" s="20"/>
       <c r="Y33" s="20"/>
@@ -3575,14 +3571,10 @@
     </row>
     <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="22" t="s">
-        <v>114</v>
-      </c>
-      <c r="B34" s="22" t="s">
-        <v>137</v>
-      </c>
-      <c r="C34" s="27" t="s">
-        <v>138</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="B34" s="22"/>
+      <c r="C34" s="20"/>
       <c r="D34" s="20"/>
       <c r="E34" s="20"/>
       <c r="F34" s="20"/>
@@ -3590,9 +3582,7 @@
       <c r="H34" s="20"/>
       <c r="I34" s="20"/>
       <c r="J34" s="20"/>
-      <c r="K34" s="20" t="s">
-        <v>34</v>
-      </c>
+      <c r="K34" s="20"/>
       <c r="L34" s="20"/>
       <c r="M34" s="20"/>
       <c r="N34" s="20"/>
@@ -3629,19 +3619,37 @@
     </row>
     <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="B35" s="22"/>
-      <c r="C35" s="20"/>
-      <c r="D35" s="20"/>
-      <c r="E35" s="20"/>
-      <c r="F35" s="20"/>
-      <c r="G35" s="20"/>
+        <v>137</v>
+      </c>
+      <c r="B35" s="22" t="s">
+        <v>138</v>
+      </c>
+      <c r="C35" s="20" t="s">
+        <v>139</v>
+      </c>
+      <c r="D35" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="E35" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="F35" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="G35" s="23" t="s">
+        <v>140</v>
+      </c>
       <c r="H35" s="20"/>
-      <c r="I35" s="20"/>
-      <c r="J35" s="20"/>
+      <c r="I35" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="J35" s="20" t="s">
+        <v>93</v>
+      </c>
       <c r="K35" s="20"/>
-      <c r="L35" s="20"/>
+      <c r="L35" s="20" t="s">
+        <v>128</v>
+      </c>
       <c r="M35" s="20"/>
       <c r="N35" s="20"/>
       <c r="O35" s="20"/>
@@ -3677,46 +3685,50 @@
     </row>
     <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="22" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="B36" s="22" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="C36" s="20" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="D36" s="23" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="E36" s="20" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="F36" s="20" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="G36" s="23" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="H36" s="20"/>
       <c r="I36" s="20" t="s">
-        <v>145</v>
-      </c>
-      <c r="J36" s="20" t="s">
-        <v>95</v>
-      </c>
+        <v>151</v>
+      </c>
+      <c r="J36" s="20"/>
       <c r="K36" s="20"/>
-      <c r="L36" s="20" t="s">
-        <v>130</v>
-      </c>
+      <c r="L36" s="20"/>
       <c r="M36" s="20"/>
-      <c r="N36" s="20"/>
-      <c r="O36" s="20"/>
-      <c r="P36" s="20"/>
+      <c r="N36" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="O36" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="P36" s="28" t="s">
+        <v>154</v>
+      </c>
       <c r="Q36" s="20"/>
       <c r="R36" s="20"/>
       <c r="S36" s="20"/>
       <c r="T36" s="20"/>
-      <c r="U36" s="20"/>
+      <c r="U36" s="20" t="s">
+        <v>155</v>
+      </c>
       <c r="V36" s="20"/>
       <c r="W36" s="20"/>
       <c r="X36" s="20"/>
@@ -3743,49 +3755,49 @@
     </row>
     <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="22" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B37" s="22" t="s">
-        <v>147</v>
+        <v>156</v>
       </c>
       <c r="C37" s="20" t="s">
-        <v>148</v>
+        <v>157</v>
       </c>
       <c r="D37" s="23" t="s">
-        <v>149</v>
+        <v>158</v>
       </c>
       <c r="E37" s="20" t="s">
-        <v>150</v>
+        <v>159</v>
       </c>
       <c r="F37" s="20" t="s">
-        <v>151</v>
+        <v>160</v>
       </c>
       <c r="G37" s="23" t="s">
-        <v>152</v>
+        <v>161</v>
       </c>
       <c r="H37" s="20"/>
       <c r="I37" s="20" t="s">
-        <v>153</v>
+        <v>162</v>
       </c>
       <c r="J37" s="20"/>
       <c r="K37" s="20"/>
       <c r="L37" s="20"/>
       <c r="M37" s="20"/>
       <c r="N37" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="O37" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="P37" s="28" t="s">
         <v>154</v>
-      </c>
-      <c r="O37" s="20" t="s">
-        <v>155</v>
-      </c>
-      <c r="P37" s="28" t="s">
-        <v>156</v>
       </c>
       <c r="Q37" s="20"/>
       <c r="R37" s="20"/>
       <c r="S37" s="20"/>
       <c r="T37" s="20"/>
       <c r="U37" s="20" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="V37" s="20"/>
       <c r="W37" s="20"/>
@@ -3813,59 +3825,63 @@
     </row>
     <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="22" t="s">
-        <v>146</v>
+        <v>163</v>
       </c>
       <c r="B38" s="22" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="C38" s="20" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="D38" s="23" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="E38" s="20" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="F38" s="20" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="G38" s="23" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="H38" s="20"/>
       <c r="I38" s="20" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="J38" s="20"/>
       <c r="K38" s="20"/>
       <c r="L38" s="20"/>
       <c r="M38" s="20"/>
-      <c r="N38" s="20" t="s">
-        <v>154</v>
-      </c>
-      <c r="O38" s="20" t="s">
-        <v>155</v>
-      </c>
-      <c r="P38" s="28" t="s">
-        <v>156</v>
-      </c>
+      <c r="N38" s="20"/>
+      <c r="O38" s="20"/>
+      <c r="P38" s="20"/>
       <c r="Q38" s="20"/>
       <c r="R38" s="20"/>
       <c r="S38" s="20"/>
       <c r="T38" s="20"/>
-      <c r="U38" s="20" t="s">
-        <v>157</v>
-      </c>
+      <c r="U38" s="20"/>
       <c r="V38" s="20"/>
       <c r="W38" s="20"/>
-      <c r="X38" s="20"/>
-      <c r="Y38" s="20"/>
-      <c r="Z38" s="20"/>
-      <c r="AA38" s="20"/>
-      <c r="AB38" s="20"/>
+      <c r="X38" s="20" t="s">
+        <v>170</v>
+      </c>
+      <c r="Y38" s="23" t="s">
+        <v>171</v>
+      </c>
+      <c r="Z38" s="20" t="s">
+        <v>172</v>
+      </c>
+      <c r="AA38" s="20" t="s">
+        <v>173</v>
+      </c>
+      <c r="AB38" s="23" t="s">
+        <v>174</v>
+      </c>
       <c r="AC38" s="20"/>
-      <c r="AD38" s="20"/>
+      <c r="AD38" s="20" t="s">
+        <v>175</v>
+      </c>
       <c r="AE38" s="20"/>
       <c r="AF38" s="20"/>
       <c r="AG38" s="20"/>
@@ -3883,32 +3899,36 @@
     </row>
     <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="22" t="s">
-        <v>165</v>
+        <v>36</v>
       </c>
       <c r="B39" s="22" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
       <c r="C39" s="20" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="D39" s="23" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
       <c r="E39" s="20" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="F39" s="20" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="G39" s="23" t="s">
-        <v>168</v>
+        <v>181</v>
       </c>
       <c r="H39" s="20"/>
       <c r="I39" s="20" t="s">
-        <v>171</v>
-      </c>
-      <c r="J39" s="20"/>
-      <c r="K39" s="20"/>
+        <v>182</v>
+      </c>
+      <c r="J39" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="K39" s="20" t="s">
+        <v>183</v>
+      </c>
       <c r="L39" s="20"/>
       <c r="M39" s="20"/>
       <c r="N39" s="20"/>
@@ -3921,25 +3941,13 @@
       <c r="U39" s="20"/>
       <c r="V39" s="20"/>
       <c r="W39" s="20"/>
-      <c r="X39" s="20" t="s">
-        <v>172</v>
-      </c>
-      <c r="Y39" s="23" t="s">
-        <v>173</v>
-      </c>
-      <c r="Z39" s="20" t="s">
-        <v>174</v>
-      </c>
-      <c r="AA39" s="20" t="s">
-        <v>175</v>
-      </c>
-      <c r="AB39" s="23" t="s">
-        <v>176</v>
-      </c>
+      <c r="X39" s="20"/>
+      <c r="Y39" s="20"/>
+      <c r="Z39" s="20"/>
+      <c r="AA39" s="20"/>
+      <c r="AB39" s="20"/>
       <c r="AC39" s="20"/>
-      <c r="AD39" s="20" t="s">
-        <v>177</v>
-      </c>
+      <c r="AD39" s="20"/>
       <c r="AE39" s="20"/>
       <c r="AF39" s="20"/>
       <c r="AG39" s="20"/>
@@ -3960,33 +3968,29 @@
         <v>36</v>
       </c>
       <c r="B40" s="22" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="C40" s="20" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="D40" s="23" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="E40" s="20" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="F40" s="20" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="G40" s="23" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="H40" s="20"/>
       <c r="I40" s="20" t="s">
-        <v>184</v>
-      </c>
-      <c r="J40" s="20" t="s">
-        <v>95</v>
-      </c>
-      <c r="K40" s="20" t="s">
-        <v>185</v>
-      </c>
+        <v>190</v>
+      </c>
+      <c r="J40" s="20"/>
+      <c r="K40" s="20"/>
       <c r="L40" s="20"/>
       <c r="M40" s="20"/>
       <c r="N40" s="20"/>
@@ -4026,22 +4030,22 @@
         <v>36</v>
       </c>
       <c r="B41" s="22" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="C41" s="20" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="D41" s="23" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="E41" s="20" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="F41" s="20" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="G41" s="23" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="H41" s="20"/>
       <c r="I41" s="20" t="s">
@@ -4049,7 +4053,9 @@
       </c>
       <c r="J41" s="20"/>
       <c r="K41" s="20"/>
-      <c r="L41" s="20"/>
+      <c r="L41" s="20" t="s">
+        <v>197</v>
+      </c>
       <c r="M41" s="20"/>
       <c r="N41" s="20"/>
       <c r="O41" s="20"/>
@@ -4085,36 +4091,30 @@
     </row>
     <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="22" t="s">
-        <v>36</v>
+        <v>198</v>
       </c>
       <c r="B42" s="22" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="C42" s="20" t="s">
-        <v>194</v>
-      </c>
-      <c r="D42" s="23" t="s">
-        <v>195</v>
-      </c>
-      <c r="E42" s="20" t="s">
-        <v>196</v>
-      </c>
-      <c r="F42" s="20" t="s">
-        <v>197</v>
-      </c>
-      <c r="G42" s="23" t="s">
-        <v>198</v>
-      </c>
+        <v>200</v>
+      </c>
+      <c r="D42" s="20"/>
+      <c r="E42" s="20"/>
+      <c r="F42" s="20"/>
+      <c r="G42" s="20"/>
       <c r="H42" s="20"/>
-      <c r="I42" s="20" t="s">
-        <v>194</v>
-      </c>
-      <c r="J42" s="20"/>
+      <c r="I42" s="20"/>
+      <c r="J42" s="20" t="s">
+        <v>93</v>
+      </c>
       <c r="K42" s="20"/>
       <c r="L42" s="20" t="s">
-        <v>199</v>
-      </c>
-      <c r="M42" s="20"/>
+        <v>69</v>
+      </c>
+      <c r="M42" s="20" t="s">
+        <v>66</v>
+      </c>
       <c r="N42" s="20"/>
       <c r="O42" s="20"/>
       <c r="P42" s="20"/>
@@ -4123,7 +4123,9 @@
       <c r="S42" s="20"/>
       <c r="T42" s="20"/>
       <c r="U42" s="20"/>
-      <c r="V42" s="20"/>
+      <c r="V42" s="20" t="s">
+        <v>201</v>
+      </c>
       <c r="W42" s="20"/>
       <c r="X42" s="20"/>
       <c r="Y42" s="20"/>
@@ -4149,30 +4151,36 @@
     </row>
     <row r="43" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="22" t="s">
-        <v>200</v>
+        <v>31</v>
       </c>
       <c r="B43" s="22" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C43" s="20" t="s">
-        <v>202</v>
-      </c>
-      <c r="D43" s="20"/>
-      <c r="E43" s="20"/>
-      <c r="F43" s="20"/>
-      <c r="G43" s="20"/>
+        <v>33</v>
+      </c>
+      <c r="D43" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="E43" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="F43" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="G43" s="20" t="s">
+        <v>33</v>
+      </c>
       <c r="H43" s="20"/>
-      <c r="I43" s="20"/>
-      <c r="J43" s="20" t="s">
-        <v>95</v>
-      </c>
+      <c r="I43" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="J43" s="20"/>
       <c r="K43" s="20"/>
       <c r="L43" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="M43" s="20" t="s">
-        <v>68</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="M43" s="20"/>
       <c r="N43" s="20"/>
       <c r="O43" s="20"/>
       <c r="P43" s="20"/>
@@ -4181,9 +4189,7 @@
       <c r="S43" s="20"/>
       <c r="T43" s="20"/>
       <c r="U43" s="20"/>
-      <c r="V43" s="20" t="s">
-        <v>203</v>
-      </c>
+      <c r="V43" s="20"/>
       <c r="W43" s="20"/>
       <c r="X43" s="20"/>
       <c r="Y43" s="20"/>
@@ -4209,35 +4215,21 @@
     </row>
     <row r="44" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="22" t="s">
-        <v>31</v>
+        <v>73</v>
       </c>
       <c r="B44" s="22" t="s">
-        <v>204</v>
-      </c>
-      <c r="C44" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="D44" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="E44" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="F44" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="G44" s="20" t="s">
-        <v>33</v>
-      </c>
+        <v>203</v>
+      </c>
+      <c r="C44" s="20"/>
+      <c r="D44" s="20"/>
+      <c r="E44" s="20"/>
+      <c r="F44" s="20"/>
+      <c r="G44" s="20"/>
       <c r="H44" s="20"/>
-      <c r="I44" s="20" t="s">
-        <v>33</v>
-      </c>
+      <c r="I44" s="20"/>
       <c r="J44" s="20"/>
       <c r="K44" s="20"/>
-      <c r="L44" s="20" t="s">
-        <v>71</v>
-      </c>
+      <c r="L44" s="20"/>
       <c r="M44" s="20"/>
       <c r="N44" s="20"/>
       <c r="O44" s="20"/>
@@ -4247,7 +4239,9 @@
       <c r="S44" s="20"/>
       <c r="T44" s="20"/>
       <c r="U44" s="20"/>
-      <c r="V44" s="20"/>
+      <c r="V44" s="20" t="s">
+        <v>204</v>
+      </c>
       <c r="W44" s="20"/>
       <c r="X44" s="20"/>
       <c r="Y44" s="20"/>
@@ -4273,7 +4267,7 @@
     </row>
     <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="22" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B45" s="22" t="s">
         <v>205</v>
@@ -4325,7 +4319,7 @@
     </row>
     <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="22" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B46" s="22" t="s">
         <v>207</v>
@@ -4377,11 +4371,9 @@
     </row>
     <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="B47" s="22" t="s">
-        <v>209</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="B47" s="22"/>
       <c r="C47" s="20"/>
       <c r="D47" s="20"/>
       <c r="E47" s="20"/>
@@ -4401,9 +4393,7 @@
       <c r="S47" s="20"/>
       <c r="T47" s="20"/>
       <c r="U47" s="20"/>
-      <c r="V47" s="20" t="s">
-        <v>210</v>
-      </c>
+      <c r="V47" s="20"/>
       <c r="W47" s="20"/>
       <c r="X47" s="20"/>
       <c r="Y47" s="20"/>
@@ -4429,7 +4419,7 @@
     </row>
     <row r="48" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="22" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B48" s="22"/>
       <c r="C48" s="20"/>
@@ -4475,54 +4465,7 @@
       <c r="AQ48" s="20"/>
       <c r="AR48" s="20"/>
     </row>
-    <row r="49" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A49" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="B49" s="22"/>
-      <c r="C49" s="20"/>
-      <c r="D49" s="20"/>
-      <c r="E49" s="20"/>
-      <c r="F49" s="20"/>
-      <c r="G49" s="20"/>
-      <c r="H49" s="20"/>
-      <c r="I49" s="20"/>
-      <c r="J49" s="20"/>
-      <c r="K49" s="20"/>
-      <c r="L49" s="20"/>
-      <c r="M49" s="20"/>
-      <c r="N49" s="20"/>
-      <c r="O49" s="20"/>
-      <c r="P49" s="20"/>
-      <c r="Q49" s="20"/>
-      <c r="R49" s="20"/>
-      <c r="S49" s="20"/>
-      <c r="T49" s="20"/>
-      <c r="U49" s="20"/>
-      <c r="V49" s="20"/>
-      <c r="W49" s="20"/>
-      <c r="X49" s="20"/>
-      <c r="Y49" s="20"/>
-      <c r="Z49" s="20"/>
-      <c r="AA49" s="20"/>
-      <c r="AB49" s="20"/>
-      <c r="AC49" s="20"/>
-      <c r="AD49" s="20"/>
-      <c r="AE49" s="20"/>
-      <c r="AF49" s="20"/>
-      <c r="AG49" s="20"/>
-      <c r="AH49" s="20"/>
-      <c r="AI49" s="20"/>
-      <c r="AJ49" s="20"/>
-      <c r="AK49" s="20"/>
-      <c r="AL49" s="20"/>
-      <c r="AM49" s="20"/>
-      <c r="AN49" s="20"/>
-      <c r="AO49" s="20"/>
-      <c r="AP49" s="20"/>
-      <c r="AQ49" s="20"/>
-      <c r="AR49" s="20"/>
-    </row>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -4546,7 +4489,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.390625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.29"/>
@@ -4563,7 +4506,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="29" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B1" s="29" t="s">
         <v>1</v>
@@ -4592,434 +4535,434 @@
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="30" t="s">
+        <v>210</v>
+      </c>
+      <c r="B2" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>211</v>
+      </c>
+      <c r="D2" s="31" t="s">
         <v>212</v>
       </c>
-      <c r="B2" s="30" t="s">
-        <v>68</v>
-      </c>
-      <c r="C2" s="30" t="s">
+      <c r="E2" s="16" t="s">
         <v>213</v>
       </c>
-      <c r="D2" s="31" t="s">
+      <c r="F2" s="17" t="s">
         <v>214</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="G2" s="32" t="s">
         <v>215</v>
-      </c>
-      <c r="F2" s="17" t="s">
-        <v>216</v>
-      </c>
-      <c r="G2" s="32" t="s">
-        <v>217</v>
       </c>
       <c r="H2" s="19"/>
       <c r="I2" s="20" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="30" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B3" s="30" t="s">
+        <v>217</v>
+      </c>
+      <c r="C3" s="30" t="s">
+        <v>218</v>
+      </c>
+      <c r="D3" s="31" t="s">
         <v>219</v>
       </c>
-      <c r="C3" s="30" t="s">
+      <c r="E3" s="16" t="s">
         <v>220</v>
       </c>
-      <c r="D3" s="31" t="s">
+      <c r="F3" s="17" t="s">
         <v>221</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="G3" s="32" t="s">
         <v>222</v>
-      </c>
-      <c r="F3" s="17" t="s">
-        <v>223</v>
-      </c>
-      <c r="G3" s="32" t="s">
-        <v>224</v>
       </c>
       <c r="H3" s="19"/>
       <c r="I3" s="20" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="30" t="s">
+        <v>224</v>
+      </c>
+      <c r="B4" s="30" t="s">
+        <v>225</v>
+      </c>
+      <c r="C4" s="30" t="s">
         <v>226</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="D4" s="33" t="s">
         <v>227</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="E4" s="16" t="s">
         <v>228</v>
       </c>
-      <c r="D4" s="33" t="s">
+      <c r="F4" s="17" t="s">
         <v>229</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="G4" s="32" t="s">
         <v>230</v>
-      </c>
-      <c r="F4" s="17" t="s">
-        <v>231</v>
-      </c>
-      <c r="G4" s="32" t="s">
-        <v>232</v>
       </c>
       <c r="H4" s="19"/>
       <c r="I4" s="20" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="30" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B5" s="30" t="s">
+        <v>232</v>
+      </c>
+      <c r="C5" s="30" t="s">
+        <v>233</v>
+      </c>
+      <c r="D5" s="33" t="s">
         <v>234</v>
       </c>
-      <c r="C5" s="30" t="s">
+      <c r="E5" s="16" t="s">
         <v>235</v>
       </c>
-      <c r="D5" s="33" t="s">
+      <c r="F5" s="17" t="s">
         <v>236</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="G5" s="32" t="s">
         <v>237</v>
-      </c>
-      <c r="F5" s="17" t="s">
-        <v>238</v>
-      </c>
-      <c r="G5" s="32" t="s">
-        <v>239</v>
       </c>
       <c r="H5" s="19"/>
       <c r="I5" s="20" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="30" t="s">
+        <v>239</v>
+      </c>
+      <c r="B6" s="30" t="s">
+        <v>225</v>
+      </c>
+      <c r="C6" s="30" t="s">
+        <v>240</v>
+      </c>
+      <c r="D6" s="33" t="s">
         <v>241</v>
       </c>
-      <c r="B6" s="30" t="s">
-        <v>227</v>
-      </c>
-      <c r="C6" s="30" t="s">
+      <c r="E6" s="16" t="s">
         <v>242</v>
       </c>
-      <c r="D6" s="33" t="s">
+      <c r="F6" s="17" t="s">
         <v>243</v>
       </c>
-      <c r="E6" s="16" t="s">
+      <c r="G6" s="32" t="s">
         <v>244</v>
-      </c>
-      <c r="F6" s="17" t="s">
-        <v>245</v>
-      </c>
-      <c r="G6" s="32" t="s">
-        <v>246</v>
       </c>
       <c r="H6" s="19"/>
       <c r="I6" s="20" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="30" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B7" s="30" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C7" s="30" t="s">
+        <v>246</v>
+      </c>
+      <c r="D7" s="33" t="s">
+        <v>247</v>
+      </c>
+      <c r="E7" s="16" t="s">
         <v>248</v>
       </c>
-      <c r="D7" s="33" t="s">
+      <c r="F7" s="17" t="s">
         <v>249</v>
       </c>
-      <c r="E7" s="16" t="s">
+      <c r="G7" s="32" t="s">
         <v>250</v>
-      </c>
-      <c r="F7" s="17" t="s">
-        <v>251</v>
-      </c>
-      <c r="G7" s="32" t="s">
-        <v>252</v>
       </c>
       <c r="H7" s="19"/>
       <c r="I7" s="20" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
+        <v>252</v>
+      </c>
+      <c r="B8" s="34" t="s">
+        <v>253</v>
+      </c>
+      <c r="C8" s="35" t="s">
         <v>254</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="D8" s="33" t="s">
         <v>255</v>
       </c>
-      <c r="C8" s="35" t="s">
+      <c r="E8" s="16" t="s">
         <v>256</v>
       </c>
-      <c r="D8" s="33" t="s">
+      <c r="F8" s="17" t="s">
         <v>257</v>
       </c>
-      <c r="E8" s="16" t="s">
+      <c r="G8" s="32" t="s">
         <v>258</v>
-      </c>
-      <c r="F8" s="17" t="s">
-        <v>259</v>
-      </c>
-      <c r="G8" s="32" t="s">
-        <v>260</v>
       </c>
       <c r="H8" s="19"/>
       <c r="I8" s="20" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
+        <v>260</v>
+      </c>
+      <c r="B9" s="34" t="s">
+        <v>261</v>
+      </c>
+      <c r="C9" s="35" t="s">
         <v>262</v>
       </c>
-      <c r="B9" s="34" t="s">
+      <c r="D9" s="33" t="s">
         <v>263</v>
       </c>
-      <c r="C9" s="35" t="s">
+      <c r="E9" s="16" t="s">
         <v>264</v>
       </c>
-      <c r="D9" s="33" t="s">
+      <c r="F9" s="17" t="s">
         <v>265</v>
       </c>
-      <c r="E9" s="16" t="s">
+      <c r="G9" s="32" t="s">
         <v>266</v>
-      </c>
-      <c r="F9" s="17" t="s">
-        <v>267</v>
-      </c>
-      <c r="G9" s="32" t="s">
-        <v>268</v>
       </c>
       <c r="H9" s="19"/>
       <c r="I9" s="20" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B10" s="34" t="s">
+        <v>268</v>
+      </c>
+      <c r="C10" s="35" t="s">
+        <v>269</v>
+      </c>
+      <c r="D10" s="33" t="s">
         <v>270</v>
       </c>
-      <c r="C10" s="35" t="s">
+      <c r="E10" s="16" t="s">
         <v>271</v>
       </c>
-      <c r="D10" s="33" t="s">
+      <c r="F10" s="17" t="s">
         <v>272</v>
       </c>
-      <c r="E10" s="16" t="s">
+      <c r="G10" s="32" t="s">
         <v>273</v>
-      </c>
-      <c r="F10" s="17" t="s">
-        <v>274</v>
-      </c>
-      <c r="G10" s="32" t="s">
-        <v>275</v>
       </c>
       <c r="H10" s="19"/>
       <c r="I10" s="20" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B11" s="34" t="s">
+        <v>275</v>
+      </c>
+      <c r="C11" s="35" t="s">
+        <v>276</v>
+      </c>
+      <c r="D11" s="33" t="s">
         <v>277</v>
       </c>
-      <c r="C11" s="35" t="s">
+      <c r="E11" s="16" t="s">
         <v>278</v>
       </c>
-      <c r="D11" s="33" t="s">
+      <c r="F11" s="17" t="s">
         <v>279</v>
       </c>
-      <c r="E11" s="16" t="s">
-        <v>280</v>
-      </c>
-      <c r="F11" s="17" t="s">
-        <v>281</v>
-      </c>
       <c r="G11" s="32" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="H11" s="19"/>
       <c r="I11" s="20" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B12" s="34" t="s">
+        <v>281</v>
+      </c>
+      <c r="C12" s="35" t="s">
+        <v>282</v>
+      </c>
+      <c r="D12" s="33" t="s">
         <v>283</v>
       </c>
-      <c r="C12" s="35" t="s">
+      <c r="E12" s="16" t="s">
         <v>284</v>
       </c>
-      <c r="D12" s="33" t="s">
+      <c r="F12" s="17" t="s">
         <v>285</v>
       </c>
-      <c r="E12" s="16" t="s">
+      <c r="G12" s="36" t="s">
         <v>286</v>
-      </c>
-      <c r="F12" s="17" t="s">
-        <v>287</v>
-      </c>
-      <c r="G12" s="36" t="s">
-        <v>288</v>
       </c>
       <c r="H12" s="19"/>
       <c r="I12" s="20" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B13" s="0" t="s">
+        <v>288</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>289</v>
+      </c>
+      <c r="D13" s="31" t="s">
         <v>290</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="E13" s="16" t="s">
         <v>291</v>
       </c>
-      <c r="D13" s="31" t="s">
+      <c r="F13" s="17" t="s">
         <v>292</v>
       </c>
-      <c r="E13" s="16" t="s">
+      <c r="G13" s="32" t="s">
         <v>293</v>
-      </c>
-      <c r="F13" s="17" t="s">
-        <v>294</v>
-      </c>
-      <c r="G13" s="32" t="s">
-        <v>295</v>
       </c>
       <c r="H13" s="19"/>
       <c r="I13" s="20" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B14" s="34" t="s">
+        <v>294</v>
+      </c>
+      <c r="C14" s="35" t="s">
+        <v>295</v>
+      </c>
+      <c r="D14" s="31" t="s">
         <v>296</v>
       </c>
-      <c r="C14" s="35" t="s">
+      <c r="E14" s="16" t="s">
         <v>297</v>
       </c>
-      <c r="D14" s="31" t="s">
+      <c r="F14" s="17" t="s">
         <v>298</v>
       </c>
-      <c r="E14" s="16" t="s">
-        <v>299</v>
-      </c>
-      <c r="F14" s="17" t="s">
-        <v>300</v>
-      </c>
       <c r="G14" s="32" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="H14" s="19"/>
       <c r="I14" s="20" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
+        <v>300</v>
+      </c>
+      <c r="B15" s="34" t="s">
+        <v>301</v>
+      </c>
+      <c r="C15" s="35" t="s">
         <v>302</v>
       </c>
-      <c r="B15" s="34" t="s">
+      <c r="D15" s="31" t="s">
         <v>303</v>
       </c>
-      <c r="C15" s="35" t="s">
+      <c r="E15" s="16" t="s">
         <v>304</v>
       </c>
-      <c r="D15" s="31" t="s">
+      <c r="F15" s="17" t="s">
         <v>305</v>
       </c>
-      <c r="E15" s="16" t="s">
+      <c r="G15" s="32" t="s">
         <v>306</v>
-      </c>
-      <c r="F15" s="17" t="s">
-        <v>307</v>
-      </c>
-      <c r="G15" s="32" t="s">
-        <v>308</v>
       </c>
       <c r="H15" s="19"/>
       <c r="I15" s="20" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B16" s="34" t="s">
+        <v>308</v>
+      </c>
+      <c r="C16" s="35" t="s">
+        <v>309</v>
+      </c>
+      <c r="D16" s="31" t="s">
         <v>310</v>
       </c>
-      <c r="C16" s="35" t="s">
+      <c r="E16" s="16" t="s">
         <v>311</v>
       </c>
-      <c r="D16" s="31" t="s">
+      <c r="F16" s="17" t="s">
         <v>312</v>
       </c>
-      <c r="E16" s="16" t="s">
+      <c r="G16" s="32" t="s">
         <v>313</v>
-      </c>
-      <c r="F16" s="17" t="s">
-        <v>314</v>
-      </c>
-      <c r="G16" s="32" t="s">
-        <v>315</v>
       </c>
       <c r="H16" s="19"/>
       <c r="I16" s="20" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B17" s="34" t="s">
+        <v>315</v>
+      </c>
+      <c r="C17" s="35" t="s">
+        <v>316</v>
+      </c>
+      <c r="D17" s="31" t="s">
         <v>317</v>
       </c>
-      <c r="C17" s="35" t="s">
+      <c r="E17" s="16" t="s">
         <v>318</v>
       </c>
-      <c r="D17" s="31" t="s">
+      <c r="F17" s="17" t="s">
         <v>319</v>
       </c>
-      <c r="E17" s="16" t="s">
-        <v>320</v>
-      </c>
-      <c r="F17" s="17" t="s">
-        <v>321</v>
-      </c>
       <c r="G17" s="32" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="H17" s="19"/>
       <c r="I17" s="20" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
   </sheetData>
@@ -5044,7 +4987,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.390625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="7.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.43"/>
@@ -5054,40 +4997,40 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>324</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>326</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C2" s="37" t="str">
         <f aca="true">TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2022-12-22  12-22</v>
+        <v>2022-12-26  12-32</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
change `should_create_user` field's type to `calculate`
</commit_message>
<xml_diff>
--- a/config/default/forms/contact/person-create.xlsx
+++ b/config/default/forms/contact/person-create.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="330">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -815,16 +815,13 @@
     <t xml:space="preserve">multiline</t>
   </si>
   <si>
-    <t xml:space="preserve">select_one yes_no</t>
-  </si>
-  <si>
     <t xml:space="preserve">should_create_user</t>
   </si>
   <si>
     <t xml:space="preserve">Create a user for this contact</t>
   </si>
   <si>
-    <t xml:space="preserve">if(selected( ${role},'chw') or selected( ${role},'chw_supervisor'), 'true', 'false')</t>
+    <t xml:space="preserve">selected( ${role},'chw') or selected( ${role},'chw_supervisor')</t>
   </si>
   <si>
     <t xml:space="preserve">meta</t>
@@ -1607,11 +1604,11 @@
   <dimension ref="A1:AR1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="V2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="S2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="V1" activeCellId="0" sqref="V1"/>
+      <selection pane="topRight" activeCell="S1" activeCellId="0" sqref="S1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="bottomRight" activeCell="V43" activeCellId="0" sqref="V43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4091,13 +4088,13 @@
     </row>
     <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="B42" s="22" t="s">
         <v>198</v>
       </c>
-      <c r="B42" s="22" t="s">
+      <c r="C42" s="20" t="s">
         <v>199</v>
-      </c>
-      <c r="C42" s="20" t="s">
-        <v>200</v>
       </c>
       <c r="D42" s="20"/>
       <c r="E42" s="20"/>
@@ -4105,16 +4102,10 @@
       <c r="G42" s="20"/>
       <c r="H42" s="20"/>
       <c r="I42" s="20"/>
-      <c r="J42" s="20" t="s">
-        <v>93</v>
-      </c>
+      <c r="J42" s="20"/>
       <c r="K42" s="20"/>
-      <c r="L42" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="M42" s="20" t="s">
-        <v>66</v>
-      </c>
+      <c r="L42" s="20"/>
+      <c r="M42" s="20"/>
       <c r="N42" s="20"/>
       <c r="O42" s="20"/>
       <c r="P42" s="20"/>
@@ -4124,7 +4115,7 @@
       <c r="T42" s="20"/>
       <c r="U42" s="20"/>
       <c r="V42" s="20" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="W42" s="20"/>
       <c r="X42" s="20"/>
@@ -4154,7 +4145,7 @@
         <v>31</v>
       </c>
       <c r="B43" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C43" s="20" t="s">
         <v>33</v>
@@ -4218,7 +4209,7 @@
         <v>73</v>
       </c>
       <c r="B44" s="22" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C44" s="20"/>
       <c r="D44" s="20"/>
@@ -4240,7 +4231,7 @@
       <c r="T44" s="20"/>
       <c r="U44" s="20"/>
       <c r="V44" s="20" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="W44" s="20"/>
       <c r="X44" s="20"/>
@@ -4270,7 +4261,7 @@
         <v>73</v>
       </c>
       <c r="B45" s="22" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C45" s="20"/>
       <c r="D45" s="20"/>
@@ -4292,7 +4283,7 @@
       <c r="T45" s="20"/>
       <c r="U45" s="20"/>
       <c r="V45" s="20" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="W45" s="20"/>
       <c r="X45" s="20"/>
@@ -4322,7 +4313,7 @@
         <v>73</v>
       </c>
       <c r="B46" s="22" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C46" s="20"/>
       <c r="D46" s="20"/>
@@ -4344,7 +4335,7 @@
       <c r="T46" s="20"/>
       <c r="U46" s="20"/>
       <c r="V46" s="20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="W46" s="20"/>
       <c r="X46" s="20"/>
@@ -4506,7 +4497,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="29" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B1" s="29" t="s">
         <v>1</v>
@@ -4535,434 +4526,434 @@
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="30" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B2" s="30" t="s">
         <v>66</v>
       </c>
       <c r="C2" s="30" t="s">
+        <v>210</v>
+      </c>
+      <c r="D2" s="31" t="s">
         <v>211</v>
       </c>
-      <c r="D2" s="31" t="s">
+      <c r="E2" s="16" t="s">
         <v>212</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="F2" s="17" t="s">
         <v>213</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="G2" s="32" t="s">
         <v>214</v>
-      </c>
-      <c r="G2" s="32" t="s">
-        <v>215</v>
       </c>
       <c r="H2" s="19"/>
       <c r="I2" s="20" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="30" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B3" s="30" t="s">
+        <v>216</v>
+      </c>
+      <c r="C3" s="30" t="s">
         <v>217</v>
       </c>
-      <c r="C3" s="30" t="s">
+      <c r="D3" s="31" t="s">
         <v>218</v>
       </c>
-      <c r="D3" s="31" t="s">
+      <c r="E3" s="16" t="s">
         <v>219</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="F3" s="17" t="s">
         <v>220</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="G3" s="32" t="s">
         <v>221</v>
-      </c>
-      <c r="G3" s="32" t="s">
-        <v>222</v>
       </c>
       <c r="H3" s="19"/>
       <c r="I3" s="20" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="30" t="s">
+        <v>223</v>
+      </c>
+      <c r="B4" s="30" t="s">
         <v>224</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="C4" s="30" t="s">
         <v>225</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="D4" s="33" t="s">
         <v>226</v>
       </c>
-      <c r="D4" s="33" t="s">
+      <c r="E4" s="16" t="s">
         <v>227</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="F4" s="17" t="s">
         <v>228</v>
       </c>
-      <c r="F4" s="17" t="s">
+      <c r="G4" s="32" t="s">
         <v>229</v>
-      </c>
-      <c r="G4" s="32" t="s">
-        <v>230</v>
       </c>
       <c r="H4" s="19"/>
       <c r="I4" s="20" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="30" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B5" s="30" t="s">
+        <v>231</v>
+      </c>
+      <c r="C5" s="30" t="s">
         <v>232</v>
       </c>
-      <c r="C5" s="30" t="s">
+      <c r="D5" s="33" t="s">
         <v>233</v>
       </c>
-      <c r="D5" s="33" t="s">
+      <c r="E5" s="16" t="s">
         <v>234</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="F5" s="17" t="s">
         <v>235</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="G5" s="32" t="s">
         <v>236</v>
-      </c>
-      <c r="G5" s="32" t="s">
-        <v>237</v>
       </c>
       <c r="H5" s="19"/>
       <c r="I5" s="20" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="30" t="s">
+        <v>238</v>
+      </c>
+      <c r="B6" s="30" t="s">
+        <v>224</v>
+      </c>
+      <c r="C6" s="30" t="s">
         <v>239</v>
       </c>
-      <c r="B6" s="30" t="s">
-        <v>225</v>
-      </c>
-      <c r="C6" s="30" t="s">
+      <c r="D6" s="33" t="s">
         <v>240</v>
       </c>
-      <c r="D6" s="33" t="s">
+      <c r="E6" s="16" t="s">
         <v>241</v>
       </c>
-      <c r="E6" s="16" t="s">
+      <c r="F6" s="17" t="s">
         <v>242</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="G6" s="32" t="s">
         <v>243</v>
-      </c>
-      <c r="G6" s="32" t="s">
-        <v>244</v>
       </c>
       <c r="H6" s="19"/>
       <c r="I6" s="20" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="30" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B7" s="30" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C7" s="30" t="s">
+        <v>245</v>
+      </c>
+      <c r="D7" s="33" t="s">
         <v>246</v>
       </c>
-      <c r="D7" s="33" t="s">
+      <c r="E7" s="16" t="s">
         <v>247</v>
       </c>
-      <c r="E7" s="16" t="s">
+      <c r="F7" s="17" t="s">
         <v>248</v>
       </c>
-      <c r="F7" s="17" t="s">
+      <c r="G7" s="32" t="s">
         <v>249</v>
-      </c>
-      <c r="G7" s="32" t="s">
-        <v>250</v>
       </c>
       <c r="H7" s="19"/>
       <c r="I7" s="20" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
+        <v>251</v>
+      </c>
+      <c r="B8" s="34" t="s">
         <v>252</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="C8" s="35" t="s">
         <v>253</v>
       </c>
-      <c r="C8" s="35" t="s">
+      <c r="D8" s="33" t="s">
         <v>254</v>
       </c>
-      <c r="D8" s="33" t="s">
+      <c r="E8" s="16" t="s">
         <v>255</v>
       </c>
-      <c r="E8" s="16" t="s">
+      <c r="F8" s="17" t="s">
         <v>256</v>
       </c>
-      <c r="F8" s="17" t="s">
+      <c r="G8" s="32" t="s">
         <v>257</v>
-      </c>
-      <c r="G8" s="32" t="s">
-        <v>258</v>
       </c>
       <c r="H8" s="19"/>
       <c r="I8" s="20" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
+        <v>259</v>
+      </c>
+      <c r="B9" s="34" t="s">
         <v>260</v>
       </c>
-      <c r="B9" s="34" t="s">
+      <c r="C9" s="35" t="s">
         <v>261</v>
       </c>
-      <c r="C9" s="35" t="s">
+      <c r="D9" s="33" t="s">
         <v>262</v>
       </c>
-      <c r="D9" s="33" t="s">
+      <c r="E9" s="16" t="s">
         <v>263</v>
       </c>
-      <c r="E9" s="16" t="s">
+      <c r="F9" s="17" t="s">
         <v>264</v>
       </c>
-      <c r="F9" s="17" t="s">
+      <c r="G9" s="32" t="s">
         <v>265</v>
-      </c>
-      <c r="G9" s="32" t="s">
-        <v>266</v>
       </c>
       <c r="H9" s="19"/>
       <c r="I9" s="20" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B10" s="34" t="s">
+        <v>267</v>
+      </c>
+      <c r="C10" s="35" t="s">
         <v>268</v>
       </c>
-      <c r="C10" s="35" t="s">
+      <c r="D10" s="33" t="s">
         <v>269</v>
       </c>
-      <c r="D10" s="33" t="s">
+      <c r="E10" s="16" t="s">
         <v>270</v>
       </c>
-      <c r="E10" s="16" t="s">
+      <c r="F10" s="17" t="s">
         <v>271</v>
       </c>
-      <c r="F10" s="17" t="s">
+      <c r="G10" s="32" t="s">
         <v>272</v>
-      </c>
-      <c r="G10" s="32" t="s">
-        <v>273</v>
       </c>
       <c r="H10" s="19"/>
       <c r="I10" s="20" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B11" s="34" t="s">
+        <v>274</v>
+      </c>
+      <c r="C11" s="35" t="s">
         <v>275</v>
       </c>
-      <c r="C11" s="35" t="s">
+      <c r="D11" s="33" t="s">
         <v>276</v>
       </c>
-      <c r="D11" s="33" t="s">
+      <c r="E11" s="16" t="s">
         <v>277</v>
       </c>
-      <c r="E11" s="16" t="s">
+      <c r="F11" s="17" t="s">
         <v>278</v>
       </c>
-      <c r="F11" s="17" t="s">
-        <v>279</v>
-      </c>
       <c r="G11" s="32" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="H11" s="19"/>
       <c r="I11" s="20" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B12" s="34" t="s">
+        <v>280</v>
+      </c>
+      <c r="C12" s="35" t="s">
         <v>281</v>
       </c>
-      <c r="C12" s="35" t="s">
+      <c r="D12" s="33" t="s">
         <v>282</v>
       </c>
-      <c r="D12" s="33" t="s">
+      <c r="E12" s="16" t="s">
         <v>283</v>
       </c>
-      <c r="E12" s="16" t="s">
+      <c r="F12" s="17" t="s">
         <v>284</v>
       </c>
-      <c r="F12" s="17" t="s">
+      <c r="G12" s="36" t="s">
         <v>285</v>
-      </c>
-      <c r="G12" s="36" t="s">
-        <v>286</v>
       </c>
       <c r="H12" s="19"/>
       <c r="I12" s="20" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B13" s="0" t="s">
+        <v>287</v>
+      </c>
+      <c r="C13" s="0" t="s">
         <v>288</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="D13" s="31" t="s">
         <v>289</v>
       </c>
-      <c r="D13" s="31" t="s">
+      <c r="E13" s="16" t="s">
         <v>290</v>
       </c>
-      <c r="E13" s="16" t="s">
+      <c r="F13" s="17" t="s">
         <v>291</v>
       </c>
-      <c r="F13" s="17" t="s">
+      <c r="G13" s="32" t="s">
         <v>292</v>
-      </c>
-      <c r="G13" s="32" t="s">
-        <v>293</v>
       </c>
       <c r="H13" s="19"/>
       <c r="I13" s="20" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B14" s="34" t="s">
+        <v>293</v>
+      </c>
+      <c r="C14" s="35" t="s">
         <v>294</v>
       </c>
-      <c r="C14" s="35" t="s">
+      <c r="D14" s="31" t="s">
         <v>295</v>
       </c>
-      <c r="D14" s="31" t="s">
+      <c r="E14" s="16" t="s">
         <v>296</v>
       </c>
-      <c r="E14" s="16" t="s">
+      <c r="F14" s="17" t="s">
         <v>297</v>
       </c>
-      <c r="F14" s="17" t="s">
-        <v>298</v>
-      </c>
       <c r="G14" s="32" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="H14" s="19"/>
       <c r="I14" s="20" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
+        <v>299</v>
+      </c>
+      <c r="B15" s="34" t="s">
         <v>300</v>
       </c>
-      <c r="B15" s="34" t="s">
+      <c r="C15" s="35" t="s">
         <v>301</v>
       </c>
-      <c r="C15" s="35" t="s">
+      <c r="D15" s="31" t="s">
         <v>302</v>
       </c>
-      <c r="D15" s="31" t="s">
+      <c r="E15" s="16" t="s">
         <v>303</v>
       </c>
-      <c r="E15" s="16" t="s">
+      <c r="F15" s="17" t="s">
         <v>304</v>
       </c>
-      <c r="F15" s="17" t="s">
+      <c r="G15" s="32" t="s">
         <v>305</v>
-      </c>
-      <c r="G15" s="32" t="s">
-        <v>306</v>
       </c>
       <c r="H15" s="19"/>
       <c r="I15" s="20" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B16" s="34" t="s">
+        <v>307</v>
+      </c>
+      <c r="C16" s="35" t="s">
         <v>308</v>
       </c>
-      <c r="C16" s="35" t="s">
+      <c r="D16" s="31" t="s">
         <v>309</v>
       </c>
-      <c r="D16" s="31" t="s">
+      <c r="E16" s="16" t="s">
         <v>310</v>
       </c>
-      <c r="E16" s="16" t="s">
+      <c r="F16" s="17" t="s">
         <v>311</v>
       </c>
-      <c r="F16" s="17" t="s">
+      <c r="G16" s="32" t="s">
         <v>312</v>
-      </c>
-      <c r="G16" s="32" t="s">
-        <v>313</v>
       </c>
       <c r="H16" s="19"/>
       <c r="I16" s="20" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B17" s="34" t="s">
+        <v>314</v>
+      </c>
+      <c r="C17" s="35" t="s">
         <v>315</v>
       </c>
-      <c r="C17" s="35" t="s">
+      <c r="D17" s="31" t="s">
         <v>316</v>
       </c>
-      <c r="D17" s="31" t="s">
+      <c r="E17" s="16" t="s">
         <v>317</v>
       </c>
-      <c r="E17" s="16" t="s">
+      <c r="F17" s="17" t="s">
         <v>318</v>
       </c>
-      <c r="F17" s="17" t="s">
-        <v>319</v>
-      </c>
       <c r="G17" s="32" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H17" s="19"/>
       <c r="I17" s="20" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
   </sheetData>
@@ -4997,40 +4988,40 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>324</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>325</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>326</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>327</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>328</v>
       </c>
       <c r="C2" s="37" t="str">
         <f aca="true">TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2022-12-26  12-32</v>
+        <v>2022-12-26  12-35</v>
       </c>
       <c r="E2" s="0" t="s">
+        <v>328</v>
+      </c>
+      <c r="F2" s="0" t="s">
         <v>329</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
rename `should_create_user` to `create_user_for_contact`
</commit_message>
<xml_diff>
--- a/config/default/forms/contact/person-create.xlsx
+++ b/config/default/forms/contact/person-create.xlsx
@@ -815,7 +815,7 @@
     <t xml:space="preserve">multiline</t>
   </si>
   <si>
-    <t xml:space="preserve">should_create_user</t>
+    <t xml:space="preserve">create_user_for_contact</t>
   </si>
   <si>
     <t xml:space="preserve">Create a user for this contact</t>
@@ -1608,10 +1608,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="S1" activeCellId="0" sqref="S1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="V43" activeCellId="0" sqref="V43"/>
+      <selection pane="bottomRight" activeCell="B43" activeCellId="0" sqref="B43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.359375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.43"/>
@@ -4480,7 +4480,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.359375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.29"/>
@@ -4978,7 +4978,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.359375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="7.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.43"/>
@@ -5015,7 +5015,7 @@
       </c>
       <c r="C2" s="37" t="str">
         <f aca="true">TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2022-12-26  12-35</v>
+        <v>2022-12-27  16-35</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>328</v>

</xml_diff>

<commit_message>
update default config's contact form `person-create` to set `user_for_contact.create = true` on the new contact doc
</commit_message>
<xml_diff>
--- a/config/default/forms/contact/person-create.xlsx
+++ b/config/default/forms/contact/person-create.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="330">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -819,9 +819,6 @@
   </si>
   <si>
     <t xml:space="preserve">create</t>
-  </si>
-  <si>
-    <t xml:space="preserve">add</t>
   </si>
   <si>
     <t xml:space="preserve">selected( ${role},'chw') or selected( ${role},'chw_supervisor')</t>
@@ -1614,17 +1611,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AR52"/>
+  <dimension ref="A1:AR1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="G8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="Y8" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="G1" activeCellId="0" sqref="G1"/>
+      <selection pane="topRight" activeCell="Y1" activeCellId="0" sqref="Y1"/>
       <selection pane="bottomLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="C43" activeCellId="0" sqref="C43:I43"/>
+      <selection pane="bottomRight" activeCell="AK43" activeCellId="0" sqref="AK43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.34375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.328125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.43"/>
@@ -4163,30 +4160,18 @@
     </row>
     <row r="43" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="B43" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="B43" s="29" t="s">
         <v>199</v>
       </c>
-      <c r="C43" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="D43" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="E43" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="F43" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="G43" s="20" t="s">
-        <v>33</v>
-      </c>
+      <c r="C43" s="20"/>
+      <c r="D43" s="20"/>
+      <c r="E43" s="20"/>
+      <c r="F43" s="20"/>
+      <c r="G43" s="20"/>
       <c r="H43" s="20"/>
-      <c r="I43" s="20" t="s">
-        <v>33</v>
-      </c>
+      <c r="I43" s="20"/>
       <c r="J43" s="20"/>
       <c r="K43" s="20"/>
       <c r="L43" s="20"/>
@@ -4199,7 +4184,9 @@
       <c r="S43" s="20"/>
       <c r="T43" s="20"/>
       <c r="U43" s="20"/>
-      <c r="V43" s="20"/>
+      <c r="V43" s="20" t="s">
+        <v>200</v>
+      </c>
       <c r="W43" s="20"/>
       <c r="X43" s="20"/>
       <c r="Y43" s="20"/>
@@ -4225,11 +4212,9 @@
     </row>
     <row r="44" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="22" t="s">
-        <v>73</v>
-      </c>
-      <c r="B44" s="22" t="s">
-        <v>200</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="B44" s="22"/>
       <c r="C44" s="20"/>
       <c r="D44" s="20"/>
       <c r="E44" s="20"/>
@@ -4249,9 +4234,7 @@
       <c r="S44" s="20"/>
       <c r="T44" s="20"/>
       <c r="U44" s="20"/>
-      <c r="V44" s="20" t="s">
-        <v>201</v>
-      </c>
+      <c r="V44" s="20"/>
       <c r="W44" s="20"/>
       <c r="X44" s="20"/>
       <c r="Y44" s="20"/>
@@ -4276,20 +4259,36 @@
       <c r="AR44" s="20"/>
     </row>
     <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="29" t="s">
-        <v>55</v>
-      </c>
-      <c r="B45" s="22"/>
-      <c r="C45" s="20"/>
-      <c r="D45" s="20"/>
-      <c r="E45" s="20"/>
-      <c r="F45" s="20"/>
-      <c r="G45" s="20"/>
+      <c r="A45" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="B45" s="22" t="s">
+        <v>201</v>
+      </c>
+      <c r="C45" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="D45" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="E45" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="F45" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="G45" s="20" t="s">
+        <v>33</v>
+      </c>
       <c r="H45" s="20"/>
-      <c r="I45" s="20"/>
+      <c r="I45" s="20" t="s">
+        <v>33</v>
+      </c>
       <c r="J45" s="20"/>
       <c r="K45" s="20"/>
-      <c r="L45" s="20"/>
+      <c r="L45" s="20" t="s">
+        <v>69</v>
+      </c>
       <c r="M45" s="20"/>
       <c r="N45" s="20"/>
       <c r="O45" s="20"/>
@@ -4324,10 +4323,12 @@
       <c r="AR45" s="20"/>
     </row>
     <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="29" t="s">
-        <v>55</v>
-      </c>
-      <c r="B46" s="22"/>
+      <c r="A46" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="B46" s="22" t="s">
+        <v>202</v>
+      </c>
       <c r="C46" s="20"/>
       <c r="D46" s="20"/>
       <c r="E46" s="20"/>
@@ -4347,7 +4348,9 @@
       <c r="S46" s="20"/>
       <c r="T46" s="20"/>
       <c r="U46" s="20"/>
-      <c r="V46" s="20"/>
+      <c r="V46" s="20" t="s">
+        <v>203</v>
+      </c>
       <c r="W46" s="20"/>
       <c r="X46" s="20"/>
       <c r="Y46" s="20"/>
@@ -4373,35 +4376,21 @@
     </row>
     <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="22" t="s">
-        <v>31</v>
+        <v>73</v>
       </c>
       <c r="B47" s="22" t="s">
-        <v>202</v>
-      </c>
-      <c r="C47" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="D47" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="E47" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="F47" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="G47" s="20" t="s">
-        <v>33</v>
-      </c>
+        <v>204</v>
+      </c>
+      <c r="C47" s="20"/>
+      <c r="D47" s="20"/>
+      <c r="E47" s="20"/>
+      <c r="F47" s="20"/>
+      <c r="G47" s="20"/>
       <c r="H47" s="20"/>
-      <c r="I47" s="20" t="s">
-        <v>33</v>
-      </c>
+      <c r="I47" s="20"/>
       <c r="J47" s="20"/>
       <c r="K47" s="20"/>
-      <c r="L47" s="20" t="s">
-        <v>69</v>
-      </c>
+      <c r="L47" s="20"/>
       <c r="M47" s="20"/>
       <c r="N47" s="20"/>
       <c r="O47" s="20"/>
@@ -4411,7 +4400,9 @@
       <c r="S47" s="20"/>
       <c r="T47" s="20"/>
       <c r="U47" s="20"/>
-      <c r="V47" s="20"/>
+      <c r="V47" s="20" t="s">
+        <v>205</v>
+      </c>
       <c r="W47" s="20"/>
       <c r="X47" s="20"/>
       <c r="Y47" s="20"/>
@@ -4440,7 +4431,7 @@
         <v>73</v>
       </c>
       <c r="B48" s="22" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="C48" s="20"/>
       <c r="D48" s="20"/>
@@ -4462,7 +4453,7 @@
       <c r="T48" s="20"/>
       <c r="U48" s="20"/>
       <c r="V48" s="20" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="W48" s="20"/>
       <c r="X48" s="20"/>
@@ -4489,11 +4480,9 @@
     </row>
     <row r="49" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="22" t="s">
-        <v>73</v>
-      </c>
-      <c r="B49" s="22" t="s">
-        <v>205</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="B49" s="22"/>
       <c r="C49" s="20"/>
       <c r="D49" s="20"/>
       <c r="E49" s="20"/>
@@ -4513,9 +4502,7 @@
       <c r="S49" s="20"/>
       <c r="T49" s="20"/>
       <c r="U49" s="20"/>
-      <c r="V49" s="20" t="s">
-        <v>206</v>
-      </c>
+      <c r="V49" s="20"/>
       <c r="W49" s="20"/>
       <c r="X49" s="20"/>
       <c r="Y49" s="20"/>
@@ -4541,11 +4528,9 @@
     </row>
     <row r="50" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="22" t="s">
-        <v>73</v>
-      </c>
-      <c r="B50" s="22" t="s">
-        <v>207</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="B50" s="22"/>
       <c r="C50" s="20"/>
       <c r="D50" s="20"/>
       <c r="E50" s="20"/>
@@ -4565,9 +4550,7 @@
       <c r="S50" s="20"/>
       <c r="T50" s="20"/>
       <c r="U50" s="20"/>
-      <c r="V50" s="20" t="s">
-        <v>208</v>
-      </c>
+      <c r="V50" s="20"/>
       <c r="W50" s="20"/>
       <c r="X50" s="20"/>
       <c r="Y50" s="20"/>
@@ -4591,102 +4574,8 @@
       <c r="AQ50" s="20"/>
       <c r="AR50" s="20"/>
     </row>
-    <row r="51" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="B51" s="22"/>
-      <c r="C51" s="20"/>
-      <c r="D51" s="20"/>
-      <c r="E51" s="20"/>
-      <c r="F51" s="20"/>
-      <c r="G51" s="20"/>
-      <c r="H51" s="20"/>
-      <c r="I51" s="20"/>
-      <c r="J51" s="20"/>
-      <c r="K51" s="20"/>
-      <c r="L51" s="20"/>
-      <c r="M51" s="20"/>
-      <c r="N51" s="20"/>
-      <c r="O51" s="20"/>
-      <c r="P51" s="20"/>
-      <c r="Q51" s="20"/>
-      <c r="R51" s="20"/>
-      <c r="S51" s="20"/>
-      <c r="T51" s="20"/>
-      <c r="U51" s="20"/>
-      <c r="V51" s="20"/>
-      <c r="W51" s="20"/>
-      <c r="X51" s="20"/>
-      <c r="Y51" s="20"/>
-      <c r="Z51" s="20"/>
-      <c r="AA51" s="20"/>
-      <c r="AB51" s="20"/>
-      <c r="AC51" s="20"/>
-      <c r="AD51" s="20"/>
-      <c r="AE51" s="20"/>
-      <c r="AF51" s="20"/>
-      <c r="AG51" s="20"/>
-      <c r="AH51" s="20"/>
-      <c r="AI51" s="20"/>
-      <c r="AJ51" s="20"/>
-      <c r="AK51" s="20"/>
-      <c r="AL51" s="20"/>
-      <c r="AM51" s="20"/>
-      <c r="AN51" s="20"/>
-      <c r="AO51" s="20"/>
-      <c r="AP51" s="20"/>
-      <c r="AQ51" s="20"/>
-      <c r="AR51" s="20"/>
-    </row>
-    <row r="52" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A52" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="B52" s="22"/>
-      <c r="C52" s="20"/>
-      <c r="D52" s="20"/>
-      <c r="E52" s="20"/>
-      <c r="F52" s="20"/>
-      <c r="G52" s="20"/>
-      <c r="H52" s="20"/>
-      <c r="I52" s="20"/>
-      <c r="J52" s="20"/>
-      <c r="K52" s="20"/>
-      <c r="L52" s="20"/>
-      <c r="M52" s="20"/>
-      <c r="N52" s="20"/>
-      <c r="O52" s="20"/>
-      <c r="P52" s="20"/>
-      <c r="Q52" s="20"/>
-      <c r="R52" s="20"/>
-      <c r="S52" s="20"/>
-      <c r="T52" s="20"/>
-      <c r="U52" s="20"/>
-      <c r="V52" s="20"/>
-      <c r="W52" s="20"/>
-      <c r="X52" s="20"/>
-      <c r="Y52" s="20"/>
-      <c r="Z52" s="20"/>
-      <c r="AA52" s="20"/>
-      <c r="AB52" s="20"/>
-      <c r="AC52" s="20"/>
-      <c r="AD52" s="20"/>
-      <c r="AE52" s="20"/>
-      <c r="AF52" s="20"/>
-      <c r="AG52" s="20"/>
-      <c r="AH52" s="20"/>
-      <c r="AI52" s="20"/>
-      <c r="AJ52" s="20"/>
-      <c r="AK52" s="20"/>
-      <c r="AL52" s="20"/>
-      <c r="AM52" s="20"/>
-      <c r="AN52" s="20"/>
-      <c r="AO52" s="20"/>
-      <c r="AP52" s="20"/>
-      <c r="AQ52" s="20"/>
-      <c r="AR52" s="20"/>
-    </row>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -4706,10 +4595,10 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="C43:I43 A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.34375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.328125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.29"/>
@@ -4726,7 +4615,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="30" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B1" s="30" t="s">
         <v>1</v>
@@ -4755,434 +4644,434 @@
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="31" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B2" s="31" t="s">
         <v>66</v>
       </c>
       <c r="C2" s="31" t="s">
+        <v>210</v>
+      </c>
+      <c r="D2" s="32" t="s">
         <v>211</v>
       </c>
-      <c r="D2" s="32" t="s">
+      <c r="E2" s="16" t="s">
         <v>212</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="F2" s="17" t="s">
         <v>213</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="G2" s="33" t="s">
         <v>214</v>
-      </c>
-      <c r="G2" s="33" t="s">
-        <v>215</v>
       </c>
       <c r="H2" s="19"/>
       <c r="I2" s="20" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="31" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B3" s="31" t="s">
+        <v>216</v>
+      </c>
+      <c r="C3" s="31" t="s">
         <v>217</v>
       </c>
-      <c r="C3" s="31" t="s">
+      <c r="D3" s="32" t="s">
         <v>218</v>
       </c>
-      <c r="D3" s="32" t="s">
+      <c r="E3" s="16" t="s">
         <v>219</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="F3" s="17" t="s">
         <v>220</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="G3" s="33" t="s">
         <v>221</v>
-      </c>
-      <c r="G3" s="33" t="s">
-        <v>222</v>
       </c>
       <c r="H3" s="19"/>
       <c r="I3" s="20" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="31" t="s">
+        <v>223</v>
+      </c>
+      <c r="B4" s="31" t="s">
         <v>224</v>
       </c>
-      <c r="B4" s="31" t="s">
+      <c r="C4" s="31" t="s">
         <v>225</v>
       </c>
-      <c r="C4" s="31" t="s">
+      <c r="D4" s="34" t="s">
         <v>226</v>
       </c>
-      <c r="D4" s="34" t="s">
+      <c r="E4" s="16" t="s">
         <v>227</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="F4" s="17" t="s">
         <v>228</v>
       </c>
-      <c r="F4" s="17" t="s">
+      <c r="G4" s="33" t="s">
         <v>229</v>
-      </c>
-      <c r="G4" s="33" t="s">
-        <v>230</v>
       </c>
       <c r="H4" s="19"/>
       <c r="I4" s="20" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="31" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B5" s="31" t="s">
+        <v>231</v>
+      </c>
+      <c r="C5" s="31" t="s">
         <v>232</v>
       </c>
-      <c r="C5" s="31" t="s">
+      <c r="D5" s="34" t="s">
         <v>233</v>
       </c>
-      <c r="D5" s="34" t="s">
+      <c r="E5" s="16" t="s">
         <v>234</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="F5" s="17" t="s">
         <v>235</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="G5" s="33" t="s">
         <v>236</v>
-      </c>
-      <c r="G5" s="33" t="s">
-        <v>237</v>
       </c>
       <c r="H5" s="19"/>
       <c r="I5" s="20" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="31" t="s">
+        <v>238</v>
+      </c>
+      <c r="B6" s="31" t="s">
+        <v>224</v>
+      </c>
+      <c r="C6" s="31" t="s">
         <v>239</v>
       </c>
-      <c r="B6" s="31" t="s">
-        <v>225</v>
-      </c>
-      <c r="C6" s="31" t="s">
+      <c r="D6" s="34" t="s">
         <v>240</v>
       </c>
-      <c r="D6" s="34" t="s">
+      <c r="E6" s="16" t="s">
         <v>241</v>
       </c>
-      <c r="E6" s="16" t="s">
+      <c r="F6" s="17" t="s">
         <v>242</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="G6" s="33" t="s">
         <v>243</v>
-      </c>
-      <c r="G6" s="33" t="s">
-        <v>244</v>
       </c>
       <c r="H6" s="19"/>
       <c r="I6" s="20" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="31" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B7" s="31" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C7" s="31" t="s">
+        <v>245</v>
+      </c>
+      <c r="D7" s="34" t="s">
         <v>246</v>
       </c>
-      <c r="D7" s="34" t="s">
+      <c r="E7" s="16" t="s">
         <v>247</v>
       </c>
-      <c r="E7" s="16" t="s">
+      <c r="F7" s="17" t="s">
         <v>248</v>
       </c>
-      <c r="F7" s="17" t="s">
+      <c r="G7" s="33" t="s">
         <v>249</v>
-      </c>
-      <c r="G7" s="33" t="s">
-        <v>250</v>
       </c>
       <c r="H7" s="19"/>
       <c r="I7" s="20" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
+        <v>251</v>
+      </c>
+      <c r="B8" s="35" t="s">
         <v>252</v>
       </c>
-      <c r="B8" s="35" t="s">
+      <c r="C8" s="36" t="s">
         <v>253</v>
       </c>
-      <c r="C8" s="36" t="s">
+      <c r="D8" s="34" t="s">
         <v>254</v>
       </c>
-      <c r="D8" s="34" t="s">
+      <c r="E8" s="16" t="s">
         <v>255</v>
       </c>
-      <c r="E8" s="16" t="s">
+      <c r="F8" s="17" t="s">
         <v>256</v>
       </c>
-      <c r="F8" s="17" t="s">
+      <c r="G8" s="33" t="s">
         <v>257</v>
-      </c>
-      <c r="G8" s="33" t="s">
-        <v>258</v>
       </c>
       <c r="H8" s="19"/>
       <c r="I8" s="20" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
+        <v>259</v>
+      </c>
+      <c r="B9" s="35" t="s">
         <v>260</v>
       </c>
-      <c r="B9" s="35" t="s">
+      <c r="C9" s="36" t="s">
         <v>261</v>
       </c>
-      <c r="C9" s="36" t="s">
+      <c r="D9" s="34" t="s">
         <v>262</v>
       </c>
-      <c r="D9" s="34" t="s">
+      <c r="E9" s="16" t="s">
         <v>263</v>
       </c>
-      <c r="E9" s="16" t="s">
+      <c r="F9" s="17" t="s">
         <v>264</v>
       </c>
-      <c r="F9" s="17" t="s">
+      <c r="G9" s="33" t="s">
         <v>265</v>
-      </c>
-      <c r="G9" s="33" t="s">
-        <v>266</v>
       </c>
       <c r="H9" s="19"/>
       <c r="I9" s="20" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B10" s="35" t="s">
+        <v>267</v>
+      </c>
+      <c r="C10" s="36" t="s">
         <v>268</v>
       </c>
-      <c r="C10" s="36" t="s">
+      <c r="D10" s="34" t="s">
         <v>269</v>
       </c>
-      <c r="D10" s="34" t="s">
+      <c r="E10" s="16" t="s">
         <v>270</v>
       </c>
-      <c r="E10" s="16" t="s">
+      <c r="F10" s="17" t="s">
         <v>271</v>
       </c>
-      <c r="F10" s="17" t="s">
+      <c r="G10" s="33" t="s">
         <v>272</v>
-      </c>
-      <c r="G10" s="33" t="s">
-        <v>273</v>
       </c>
       <c r="H10" s="19"/>
       <c r="I10" s="20" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B11" s="35" t="s">
+        <v>274</v>
+      </c>
+      <c r="C11" s="36" t="s">
         <v>275</v>
       </c>
-      <c r="C11" s="36" t="s">
+      <c r="D11" s="34" t="s">
         <v>276</v>
       </c>
-      <c r="D11" s="34" t="s">
+      <c r="E11" s="16" t="s">
         <v>277</v>
       </c>
-      <c r="E11" s="16" t="s">
+      <c r="F11" s="17" t="s">
         <v>278</v>
       </c>
-      <c r="F11" s="17" t="s">
-        <v>279</v>
-      </c>
       <c r="G11" s="33" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="H11" s="19"/>
       <c r="I11" s="20" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B12" s="35" t="s">
+        <v>280</v>
+      </c>
+      <c r="C12" s="36" t="s">
         <v>281</v>
       </c>
-      <c r="C12" s="36" t="s">
+      <c r="D12" s="34" t="s">
         <v>282</v>
       </c>
-      <c r="D12" s="34" t="s">
+      <c r="E12" s="16" t="s">
         <v>283</v>
       </c>
-      <c r="E12" s="16" t="s">
+      <c r="F12" s="17" t="s">
         <v>284</v>
       </c>
-      <c r="F12" s="17" t="s">
+      <c r="G12" s="37" t="s">
         <v>285</v>
-      </c>
-      <c r="G12" s="37" t="s">
-        <v>286</v>
       </c>
       <c r="H12" s="19"/>
       <c r="I12" s="20" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B13" s="0" t="s">
+        <v>287</v>
+      </c>
+      <c r="C13" s="0" t="s">
         <v>288</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="D13" s="32" t="s">
         <v>289</v>
       </c>
-      <c r="D13" s="32" t="s">
+      <c r="E13" s="16" t="s">
         <v>290</v>
       </c>
-      <c r="E13" s="16" t="s">
+      <c r="F13" s="17" t="s">
         <v>291</v>
       </c>
-      <c r="F13" s="17" t="s">
+      <c r="G13" s="33" t="s">
         <v>292</v>
-      </c>
-      <c r="G13" s="33" t="s">
-        <v>293</v>
       </c>
       <c r="H13" s="19"/>
       <c r="I13" s="20" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B14" s="35" t="s">
+        <v>293</v>
+      </c>
+      <c r="C14" s="36" t="s">
         <v>294</v>
       </c>
-      <c r="C14" s="36" t="s">
+      <c r="D14" s="32" t="s">
         <v>295</v>
       </c>
-      <c r="D14" s="32" t="s">
+      <c r="E14" s="16" t="s">
         <v>296</v>
       </c>
-      <c r="E14" s="16" t="s">
+      <c r="F14" s="17" t="s">
         <v>297</v>
       </c>
-      <c r="F14" s="17" t="s">
-        <v>298</v>
-      </c>
       <c r="G14" s="33" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="H14" s="19"/>
       <c r="I14" s="20" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
+        <v>299</v>
+      </c>
+      <c r="B15" s="35" t="s">
         <v>300</v>
       </c>
-      <c r="B15" s="35" t="s">
+      <c r="C15" s="36" t="s">
         <v>301</v>
       </c>
-      <c r="C15" s="36" t="s">
+      <c r="D15" s="32" t="s">
         <v>302</v>
       </c>
-      <c r="D15" s="32" t="s">
+      <c r="E15" s="16" t="s">
         <v>303</v>
       </c>
-      <c r="E15" s="16" t="s">
+      <c r="F15" s="17" t="s">
         <v>304</v>
       </c>
-      <c r="F15" s="17" t="s">
+      <c r="G15" s="33" t="s">
         <v>305</v>
-      </c>
-      <c r="G15" s="33" t="s">
-        <v>306</v>
       </c>
       <c r="H15" s="19"/>
       <c r="I15" s="20" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B16" s="35" t="s">
+        <v>307</v>
+      </c>
+      <c r="C16" s="36" t="s">
         <v>308</v>
       </c>
-      <c r="C16" s="36" t="s">
+      <c r="D16" s="32" t="s">
         <v>309</v>
       </c>
-      <c r="D16" s="32" t="s">
+      <c r="E16" s="16" t="s">
         <v>310</v>
       </c>
-      <c r="E16" s="16" t="s">
+      <c r="F16" s="17" t="s">
         <v>311</v>
       </c>
-      <c r="F16" s="17" t="s">
+      <c r="G16" s="33" t="s">
         <v>312</v>
-      </c>
-      <c r="G16" s="33" t="s">
-        <v>313</v>
       </c>
       <c r="H16" s="19"/>
       <c r="I16" s="20" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B17" s="35" t="s">
+        <v>314</v>
+      </c>
+      <c r="C17" s="36" t="s">
         <v>315</v>
       </c>
-      <c r="C17" s="36" t="s">
+      <c r="D17" s="32" t="s">
         <v>316</v>
       </c>
-      <c r="D17" s="32" t="s">
+      <c r="E17" s="16" t="s">
         <v>317</v>
       </c>
-      <c r="E17" s="16" t="s">
+      <c r="F17" s="17" t="s">
         <v>318</v>
       </c>
-      <c r="F17" s="17" t="s">
-        <v>319</v>
-      </c>
       <c r="G17" s="33" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H17" s="19"/>
       <c r="I17" s="20" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
   </sheetData>
@@ -5204,10 +5093,10 @@
   <dimension ref="A1:F1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C43:I43 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.34375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.328125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="7.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.43"/>
@@ -5217,40 +5106,40 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>324</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>325</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>326</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>327</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>328</v>
       </c>
       <c r="C2" s="38" t="str">
         <f aca="true">TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2023-01-18  11-30</v>
+        <v>2023-01-24  11-05</v>
       </c>
       <c r="E2" s="0" t="s">
+        <v>328</v>
+      </c>
+      <c r="F2" s="0" t="s">
         <v>329</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>